<commit_message>
Updated Forms and Records
Added field labels validation for both Records and Forms Module
</commit_message>
<xml_diff>
--- a/UTP_FormsModule.xlsx
+++ b/UTP_FormsModule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-408" yWindow="912" windowWidth="20736" windowHeight="6828" activeTab="1"/>
+    <workbookView xWindow="-408" yWindow="972" windowWidth="20736" windowHeight="6768" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary_Appendix" sheetId="4" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Funtional Unit Test" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'UI Unit Test'!$A$7:$K$152</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'UI Unit Test'!$A$7:$K$160</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="385">
   <si>
     <t>Project Name</t>
   </si>
@@ -642,15 +642,9 @@
     <t>System should return the user to create Forms Module screen where user can modify and save the forms module.</t>
   </si>
   <si>
-    <t>Form Module Tab</t>
-  </si>
-  <si>
     <t>Tab title</t>
   </si>
   <si>
-    <t>The text "Form Module" should be displayed as Tab title</t>
-  </si>
-  <si>
     <t>Create Form Module title</t>
   </si>
   <si>
@@ -846,12 +840,6 @@
     <t>Label for code_type_lang should be displayed as "code_type_lang"</t>
   </si>
   <si>
-    <t>Form tab title label validation</t>
-  </si>
-  <si>
-    <t>Create Fomrs Module form header validation</t>
-  </si>
-  <si>
     <t>date_eff_prod</t>
   </si>
   <si>
@@ -1014,9 +1002,6 @@
     <t>Sidebar link</t>
   </si>
   <si>
-    <t>Form tab sidebar links label validation</t>
-  </si>
-  <si>
     <t>The text "Create Forms Module Entry" should be displayed in sidebar of the Forms Module tab</t>
   </si>
   <si>
@@ -1069,6 +1054,186 @@
   </si>
   <si>
     <t>Text  "Search" should be displayed as label for button</t>
+  </si>
+  <si>
+    <t>The text "Forms Module" should be displayed as Tab title</t>
+  </si>
+  <si>
+    <t>Forms module tab title label validation</t>
+  </si>
+  <si>
+    <t>Forms module tab sidebar links label validation</t>
+  </si>
+  <si>
+    <t>Forms Module Tab</t>
+  </si>
+  <si>
+    <t>Create Forms Module form header validation</t>
+  </si>
+  <si>
+    <t>Forms Module tab sidebar links label validation</t>
+  </si>
+  <si>
+    <t>User is at view/modify Forms Module screen of Forms Module Tab.</t>
+  </si>
+  <si>
+    <t>num_id_chnl(s) label</t>
+  </si>
+  <si>
+    <t>num_id_chnl(s) required field</t>
+  </si>
+  <si>
+    <t>num_id_chnl(s) field type</t>
+  </si>
+  <si>
+    <t>code_type_lang label</t>
+  </si>
+  <si>
+    <t>code_type_lang required field</t>
+  </si>
+  <si>
+    <t>code_type_lang field type</t>
+  </si>
+  <si>
+    <t>date_eff_prod label</t>
+  </si>
+  <si>
+    <t>date_eff_prod required field</t>
+  </si>
+  <si>
+    <t>date_eff_prod field type</t>
+  </si>
+  <si>
+    <t>date_eff_prod value folmat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_termn_prod label </t>
+  </si>
+  <si>
+    <t>date_termn_prod required field</t>
+  </si>
+  <si>
+    <t>date_termn_prod field type</t>
+  </si>
+  <si>
+    <t>date_termn_prod values fomat</t>
+  </si>
+  <si>
+    <t>num_reqre_full label</t>
+  </si>
+  <si>
+    <t>num_reqre_full required field</t>
+  </si>
+  <si>
+    <t>num_reqre_full values format</t>
+  </si>
+  <si>
+    <t>num_reqre_full length</t>
+  </si>
+  <si>
+    <t>The user should not be able to enter more than 100 characters in the "num_reqre_full" field</t>
+  </si>
+  <si>
+    <t>The "num_reqre_full" field should accept alphanumeric and special characters</t>
+  </si>
+  <si>
+    <t>num_reqre label</t>
+  </si>
+  <si>
+    <t>num_reqre reqired field</t>
+  </si>
+  <si>
+    <t>num_reqre values format</t>
+  </si>
+  <si>
+    <t>num_reqre length</t>
+  </si>
+  <si>
+    <t>The "num_reqre" field should accept alphanumeric and special characters</t>
+  </si>
+  <si>
+    <t>The user should not be able to enter more than 20 characters in the "num_reqre" field</t>
+  </si>
+  <si>
+    <t>name_reqre label</t>
+  </si>
+  <si>
+    <t>name_reqre required field</t>
+  </si>
+  <si>
+    <t>name_reqre values format</t>
+  </si>
+  <si>
+    <t>name_reqre length</t>
+  </si>
+  <si>
+    <t>The "name_reqre" field should accept alphanumeric and special characters</t>
+  </si>
+  <si>
+    <t>The user should not be able to enter more than 60 characters in the "name_reqre" field</t>
+  </si>
+  <si>
+    <t>desc_reqre label</t>
+  </si>
+  <si>
+    <t>desc_reqre required field</t>
+  </si>
+  <si>
+    <t>desc_reqre values format</t>
+  </si>
+  <si>
+    <t>desc_reqre length</t>
+  </si>
+  <si>
+    <t>The "desc_reqre" field should accept alphanumeric and special characters</t>
+  </si>
+  <si>
+    <t>The user should not be able to enter more than 30 characters in the "desc_reqre" field</t>
+  </si>
+  <si>
+    <t>code_clast_sub_reqre label</t>
+  </si>
+  <si>
+    <t>code_clast_sub_reqre required field</t>
+  </si>
+  <si>
+    <t>code_clast_sub_reqre field type</t>
+  </si>
+  <si>
+    <t>code_clast_reqre label</t>
+  </si>
+  <si>
+    <t>code_clast_reqre required field</t>
+  </si>
+  <si>
+    <t>code_clast_reqre field type</t>
+  </si>
+  <si>
+    <t>code_type_state field type</t>
+  </si>
+  <si>
+    <t>code_type_state required field</t>
+  </si>
+  <si>
+    <t>code_type_state label</t>
+  </si>
+  <si>
+    <t>code_prod(s) label</t>
+  </si>
+  <si>
+    <t>code_prod(s) required field</t>
+  </si>
+  <si>
+    <t>code_prod(s) field type</t>
+  </si>
+  <si>
+    <t>code_abbrv_state(s) label</t>
+  </si>
+  <si>
+    <t>code_abbrv_state(s) required field</t>
+  </si>
+  <si>
+    <t>code_abbrv_state(s) field type</t>
   </si>
 </sst>
 </file>
@@ -1543,6 +1708,48 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1628,48 +1835,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2022,11 +2187,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K152"/>
+  <dimension ref="A1:K160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C86" sqref="C86"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2034,7 +2199,7 @@
     <col min="1" max="1" width="9.109375" customWidth="1"/>
     <col min="2" max="2" width="18.88671875" customWidth="1"/>
     <col min="3" max="3" width="23.44140625" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="105" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="33.109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="37" style="4" customWidth="1"/>
@@ -2045,109 +2210,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
     </row>
     <row r="2" spans="1:11" ht="15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
     </row>
     <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="70" t="s">
+      <c r="B3" s="84"/>
+      <c r="C3" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="70"/>
+      <c r="D3" s="86"/>
       <c r="E3" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
     </row>
     <row r="4" spans="1:11" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="71" t="s">
+      <c r="B4" s="85"/>
+      <c r="C4" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="71"/>
+      <c r="D4" s="87"/>
       <c r="E4" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
     </row>
     <row r="5" spans="1:11" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="71" t="s">
+      <c r="B5" s="85"/>
+      <c r="C5" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="71"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="75"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="91"/>
     </row>
     <row r="6" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="61"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="61" t="s">
+      <c r="A6" s="77"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="66" t="s">
+      <c r="D6" s="78"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="67"/>
-      <c r="H6" s="65" t="s">
+      <c r="G6" s="83"/>
+      <c r="H6" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
       <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2157,13 +2322,13 @@
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="63" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="99" t="s">
+      <c r="E7" s="69" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -2192,13 +2357,13 @@
       <c r="B8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="94" t="s">
+      <c r="C8" s="64" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="100" t="s">
+      <c r="E8" s="70" t="s">
         <v>27</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -2227,13 +2392,13 @@
       <c r="B9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="95" t="s">
+      <c r="C9" s="65" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="101" t="s">
+      <c r="E9" s="71" t="s">
         <v>46</v>
       </c>
       <c r="F9" s="8" t="s">
@@ -2253,13 +2418,13 @@
       <c r="B10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="95" t="s">
+      <c r="C10" s="65" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="71" t="s">
         <v>99</v>
       </c>
       <c r="F10" s="8" t="s">
@@ -2279,13 +2444,13 @@
       <c r="B11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="65" t="s">
         <v>45</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="101" t="s">
+      <c r="E11" s="71" t="s">
         <v>46</v>
       </c>
       <c r="F11" s="8" t="s">
@@ -2307,13 +2472,13 @@
       <c r="B12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="65" t="s">
         <v>102</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="101" t="s">
+      <c r="E12" s="71" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="8" t="s">
@@ -2333,13 +2498,13 @@
       <c r="B13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="65" t="s">
         <v>102</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E13" s="101" t="s">
+      <c r="E13" s="71" t="s">
         <v>99</v>
       </c>
       <c r="F13" s="8" t="s">
@@ -2359,13 +2524,13 @@
       <c r="B14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="95" t="s">
+      <c r="C14" s="65" t="s">
         <v>102</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E14" s="101" t="s">
+      <c r="E14" s="71" t="s">
         <v>46</v>
       </c>
       <c r="F14" s="8" t="s">
@@ -2387,13 +2552,13 @@
       <c r="B15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="65" t="s">
         <v>106</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="101" t="s">
+      <c r="E15" s="71" t="s">
         <v>46</v>
       </c>
       <c r="F15" s="8" t="s">
@@ -2413,13 +2578,13 @@
       <c r="B16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="95" t="s">
+      <c r="C16" s="65" t="s">
         <v>106</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="E16" s="101" t="s">
+      <c r="E16" s="71" t="s">
         <v>99</v>
       </c>
       <c r="F16" s="8" t="s">
@@ -2439,13 +2604,13 @@
       <c r="B17" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="95" t="s">
+      <c r="C17" s="65" t="s">
         <v>106</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="101" t="s">
+      <c r="E17" s="71" t="s">
         <v>46</v>
       </c>
       <c r="F17" s="8" t="s">
@@ -2467,13 +2632,13 @@
       <c r="B18" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="96" t="s">
+      <c r="C18" s="66" t="s">
         <v>85</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="102" t="s">
+      <c r="E18" s="72" t="s">
         <v>72</v>
       </c>
       <c r="F18" s="30" t="s">
@@ -2493,13 +2658,13 @@
       <c r="B19" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="96" t="s">
+      <c r="C19" s="66" t="s">
         <v>79</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="102" t="s">
+      <c r="E19" s="72" t="s">
         <v>72</v>
       </c>
       <c r="F19" s="30" t="s">
@@ -2515,9 +2680,9 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="95"/>
+      <c r="C20" s="65"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="101"/>
+      <c r="E20" s="71"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -2525,1707 +2690,1799 @@
       <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="106">
+      <c r="A21" s="76">
         <v>12</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="C21" s="68" t="s">
         <v>187</v>
       </c>
-      <c r="C21" s="98" t="s">
-        <v>188</v>
-      </c>
       <c r="D21" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="E21" s="101" t="s">
+        <v>326</v>
+      </c>
+      <c r="E21" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8" t="s">
-        <v>189</v>
+        <v>325</v>
       </c>
       <c r="H21" s="8"/>
       <c r="J21" s="7"/>
       <c r="K21" s="8"/>
     </row>
     <row r="22" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="106">
+      <c r="A22" s="76">
         <v>13</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C22" s="98" t="s">
-        <v>310</v>
+        <v>328</v>
+      </c>
+      <c r="C22" s="68" t="s">
+        <v>306</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E22" s="101" t="s">
+        <v>327</v>
+      </c>
+      <c r="E22" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="H22" s="8"/>
       <c r="J22" s="7"/>
       <c r="K22" s="8"/>
     </row>
     <row r="23" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="106">
+      <c r="A23" s="76">
         <v>14</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C23" s="98" t="s">
-        <v>310</v>
+        <v>328</v>
+      </c>
+      <c r="C23" s="68" t="s">
+        <v>306</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E23" s="101" t="s">
+        <v>327</v>
+      </c>
+      <c r="E23" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="H23" s="8"/>
       <c r="J23" s="7"/>
       <c r="K23" s="8"/>
     </row>
     <row r="24" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="106">
+      <c r="A24" s="76">
         <v>15</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C24" s="98" t="s">
-        <v>310</v>
+        <v>328</v>
+      </c>
+      <c r="C24" s="68" t="s">
+        <v>306</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E24" s="101" t="s">
+        <v>327</v>
+      </c>
+      <c r="E24" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="H24" s="8"/>
       <c r="J24" s="7"/>
       <c r="K24" s="8"/>
     </row>
     <row r="25" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="106">
+      <c r="A25" s="76">
         <v>16</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C25" s="98" t="s">
-        <v>310</v>
+        <v>328</v>
+      </c>
+      <c r="C25" s="68" t="s">
+        <v>306</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="E25" s="101" t="s">
+        <v>330</v>
+      </c>
+      <c r="E25" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="H25" s="8"/>
       <c r="J25" s="7"/>
       <c r="K25" s="8"/>
     </row>
     <row r="26" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="106">
+      <c r="A26" s="76">
         <v>17</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C26" s="98" t="s">
-        <v>190</v>
+        <v>328</v>
+      </c>
+      <c r="C26" s="68" t="s">
+        <v>188</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="E26" s="101" t="s">
+        <v>329</v>
+      </c>
+      <c r="E26" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H26" s="8"/>
       <c r="J26" s="7"/>
       <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="106">
+      <c r="A27" s="76">
         <v>18</v>
       </c>
       <c r="B27" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C27" s="68" t="s">
+        <v>197</v>
+      </c>
+      <c r="D27" s="74" t="s">
         <v>198</v>
       </c>
-      <c r="C27" s="98" t="s">
-        <v>199</v>
-      </c>
-      <c r="D27" s="104" t="s">
-        <v>200</v>
-      </c>
-      <c r="E27" s="101" t="s">
+      <c r="E27" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H27" s="8"/>
-      <c r="J27" s="92"/>
-      <c r="K27" s="91"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="61"/>
     </row>
     <row r="28" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="106">
+      <c r="A28" s="76">
         <v>19</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C28" s="98" t="s">
-        <v>193</v>
-      </c>
-      <c r="D28" s="104" t="s">
-        <v>196</v>
-      </c>
-      <c r="E28" s="101" t="s">
+      <c r="B28" s="68" t="s">
+        <v>191</v>
+      </c>
+      <c r="C28" s="68" t="s">
+        <v>352</v>
+      </c>
+      <c r="D28" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="E28" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H28" s="8"/>
-      <c r="J28" s="92"/>
-      <c r="K28" s="91"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="61"/>
     </row>
     <row r="29" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="106">
+      <c r="A29" s="76">
         <v>20</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C29" s="98" t="s">
-        <v>193</v>
-      </c>
-      <c r="D29" s="104" t="s">
-        <v>194</v>
-      </c>
-      <c r="E29" s="101" t="s">
+      <c r="B29" s="68" t="s">
+        <v>191</v>
+      </c>
+      <c r="C29" s="68" t="s">
+        <v>353</v>
+      </c>
+      <c r="D29" s="74" t="s">
+        <v>192</v>
+      </c>
+      <c r="E29" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H29" s="8"/>
-      <c r="J29" s="92"/>
-      <c r="K29" s="91"/>
-    </row>
-    <row r="30" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="106">
+      <c r="J29" s="62"/>
+      <c r="K29" s="61"/>
+    </row>
+    <row r="30" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="76">
+        <v>25</v>
+      </c>
+      <c r="B30" s="68" t="s">
+        <v>191</v>
+      </c>
+      <c r="C30" s="68" t="s">
+        <v>354</v>
+      </c>
+      <c r="D30" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="E30" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="44" t="s">
+        <v>356</v>
+      </c>
+      <c r="H30" s="8"/>
+      <c r="J30" s="62"/>
+      <c r="K30" s="61"/>
+    </row>
+    <row r="31" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="76">
+        <v>26</v>
+      </c>
+      <c r="B31" s="68" t="s">
+        <v>191</v>
+      </c>
+      <c r="C31" s="68" t="s">
+        <v>355</v>
+      </c>
+      <c r="D31" s="74" t="s">
+        <v>192</v>
+      </c>
+      <c r="E31" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="44" t="s">
+        <v>357</v>
+      </c>
+      <c r="H31" s="8"/>
+      <c r="J31" s="62"/>
+      <c r="K31" s="61"/>
+    </row>
+    <row r="32" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="76">
         <v>21</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C30" s="98" t="s">
-        <v>201</v>
-      </c>
-      <c r="D30" s="104" t="s">
-        <v>202</v>
-      </c>
-      <c r="E30" s="101" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="H30" s="8"/>
-      <c r="J30" s="92"/>
-      <c r="K30" s="91"/>
-    </row>
-    <row r="31" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="106">
-        <v>22</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C31" s="98" t="s">
-        <v>201</v>
-      </c>
-      <c r="D31" s="104" t="s">
-        <v>203</v>
-      </c>
-      <c r="E31" s="101" t="s">
-        <v>72</v>
-      </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="H31" s="8"/>
-      <c r="J31" s="92"/>
-      <c r="K31" s="91"/>
-    </row>
-    <row r="32" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="106">
-        <v>23</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C32" s="98" t="s">
-        <v>205</v>
-      </c>
-      <c r="D32" s="104" t="s">
-        <v>207</v>
-      </c>
-      <c r="E32" s="101" t="s">
+      <c r="B32" s="68" t="s">
+        <v>199</v>
+      </c>
+      <c r="C32" s="68" t="s">
+        <v>358</v>
+      </c>
+      <c r="D32" s="74" t="s">
+        <v>200</v>
+      </c>
+      <c r="E32" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="8" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="H32" s="8"/>
-      <c r="J32" s="92"/>
-      <c r="K32" s="91"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="61"/>
     </row>
     <row r="33" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="106">
-        <v>24</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C33" s="98" t="s">
-        <v>205</v>
-      </c>
-      <c r="D33" s="104" t="s">
-        <v>208</v>
-      </c>
-      <c r="E33" s="101" t="s">
+      <c r="A33" s="76">
+        <v>22</v>
+      </c>
+      <c r="B33" s="68" t="s">
+        <v>199</v>
+      </c>
+      <c r="C33" s="68" t="s">
+        <v>359</v>
+      </c>
+      <c r="D33" s="74" t="s">
+        <v>201</v>
+      </c>
+      <c r="E33" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H33" s="8"/>
-      <c r="J33" s="92"/>
-      <c r="K33" s="91"/>
-    </row>
-    <row r="34" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="106">
+      <c r="J33" s="62"/>
+      <c r="K33" s="61"/>
+    </row>
+    <row r="34" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="76">
         <v>25</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C34" s="98" t="s">
-        <v>206</v>
-      </c>
-      <c r="D34" s="104" t="s">
-        <v>210</v>
-      </c>
-      <c r="E34" s="101" t="s">
+      <c r="B34" s="68" t="s">
+        <v>199</v>
+      </c>
+      <c r="C34" s="68" t="s">
+        <v>360</v>
+      </c>
+      <c r="D34" s="74" t="s">
+        <v>200</v>
+      </c>
+      <c r="E34" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F34" s="8"/>
-      <c r="G34" s="8" t="s">
-        <v>224</v>
+      <c r="G34" s="44" t="s">
+        <v>362</v>
       </c>
       <c r="H34" s="8"/>
-      <c r="J34" s="92"/>
-      <c r="K34" s="91"/>
-    </row>
-    <row r="35" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="106">
+      <c r="J34" s="62"/>
+      <c r="K34" s="61"/>
+    </row>
+    <row r="35" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="76">
         <v>26</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C35" s="98" t="s">
-        <v>206</v>
-      </c>
-      <c r="D35" s="104" t="s">
-        <v>211</v>
-      </c>
-      <c r="E35" s="101" t="s">
+      <c r="B35" s="68" t="s">
+        <v>199</v>
+      </c>
+      <c r="C35" s="68" t="s">
+        <v>361</v>
+      </c>
+      <c r="D35" s="74" t="s">
+        <v>201</v>
+      </c>
+      <c r="E35" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F35" s="8"/>
-      <c r="G35" s="8" t="s">
-        <v>195</v>
+      <c r="G35" s="44" t="s">
+        <v>363</v>
       </c>
       <c r="H35" s="8"/>
-      <c r="J35" s="92"/>
-      <c r="K35" s="91"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="61"/>
     </row>
     <row r="36" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="106">
-        <v>27</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C36" s="98" t="s">
-        <v>213</v>
-      </c>
-      <c r="D36" s="104" t="s">
-        <v>200</v>
-      </c>
-      <c r="E36" s="101" t="s">
+      <c r="A36" s="76">
+        <v>23</v>
+      </c>
+      <c r="B36" s="68" t="s">
+        <v>203</v>
+      </c>
+      <c r="C36" s="68" t="s">
+        <v>364</v>
+      </c>
+      <c r="D36" s="74" t="s">
+        <v>205</v>
+      </c>
+      <c r="E36" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="8" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="H36" s="8"/>
-      <c r="J36" s="92"/>
-      <c r="K36" s="91"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="61"/>
     </row>
     <row r="37" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="106">
-        <v>28</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C37" s="98" t="s">
-        <v>214</v>
-      </c>
-      <c r="D37" s="104" t="s">
-        <v>215</v>
-      </c>
-      <c r="E37" s="101" t="s">
+      <c r="A37" s="76">
+        <v>24</v>
+      </c>
+      <c r="B37" s="68" t="s">
+        <v>203</v>
+      </c>
+      <c r="C37" s="68" t="s">
+        <v>365</v>
+      </c>
+      <c r="D37" s="74" t="s">
+        <v>206</v>
+      </c>
+      <c r="E37" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="8" t="s">
-        <v>226</v>
+        <v>193</v>
       </c>
       <c r="H37" s="8"/>
-      <c r="J37" s="92"/>
-      <c r="K37" s="91"/>
-    </row>
-    <row r="38" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="106">
-        <v>29</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C38" s="98" t="s">
-        <v>214</v>
-      </c>
-      <c r="D38" s="104" t="s">
-        <v>216</v>
-      </c>
-      <c r="E38" s="101" t="s">
+      <c r="J37" s="62"/>
+      <c r="K37" s="61"/>
+    </row>
+    <row r="38" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="76">
+        <v>25</v>
+      </c>
+      <c r="B38" s="68" t="s">
+        <v>203</v>
+      </c>
+      <c r="C38" s="68" t="s">
+        <v>366</v>
+      </c>
+      <c r="D38" s="74" t="s">
+        <v>205</v>
+      </c>
+      <c r="E38" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F38" s="8"/>
-      <c r="G38" s="8" t="s">
-        <v>195</v>
+      <c r="G38" s="44" t="s">
+        <v>368</v>
       </c>
       <c r="H38" s="8"/>
-      <c r="J38" s="92"/>
-      <c r="K38" s="91"/>
-    </row>
-    <row r="39" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="106">
-        <v>30</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C39" s="98" t="s">
-        <v>214</v>
-      </c>
-      <c r="D39" s="104" t="s">
-        <v>217</v>
-      </c>
-      <c r="E39" s="101" t="s">
+      <c r="J38" s="62"/>
+      <c r="K38" s="61"/>
+    </row>
+    <row r="39" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="76">
+        <v>26</v>
+      </c>
+      <c r="B39" s="68" t="s">
+        <v>203</v>
+      </c>
+      <c r="C39" s="68" t="s">
+        <v>367</v>
+      </c>
+      <c r="D39" s="74" t="s">
+        <v>206</v>
+      </c>
+      <c r="E39" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F39" s="8"/>
-      <c r="G39" s="8" t="s">
-        <v>227</v>
+      <c r="G39" s="44" t="s">
+        <v>369</v>
       </c>
       <c r="H39" s="8"/>
-      <c r="J39" s="92"/>
-      <c r="K39" s="91"/>
+      <c r="J39" s="62"/>
+      <c r="K39" s="61"/>
     </row>
     <row r="40" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="106">
-        <v>31</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C40" s="98" t="s">
-        <v>219</v>
-      </c>
-      <c r="D40" s="104" t="s">
-        <v>220</v>
-      </c>
-      <c r="E40" s="101" t="s">
+      <c r="A40" s="76">
+        <v>25</v>
+      </c>
+      <c r="B40" s="68" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" s="68" t="s">
+        <v>346</v>
+      </c>
+      <c r="D40" s="74" t="s">
+        <v>208</v>
+      </c>
+      <c r="E40" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H40" s="8"/>
-      <c r="J40" s="92"/>
-      <c r="K40" s="91"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="61"/>
     </row>
     <row r="41" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="106">
-        <v>32</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C41" s="98" t="s">
-        <v>222</v>
-      </c>
-      <c r="D41" s="104" t="s">
-        <v>223</v>
-      </c>
-      <c r="E41" s="101" t="s">
+      <c r="A41" s="76">
+        <v>26</v>
+      </c>
+      <c r="B41" s="68" t="s">
+        <v>204</v>
+      </c>
+      <c r="C41" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="D41" s="74" t="s">
+        <v>209</v>
+      </c>
+      <c r="E41" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="8" t="s">
-        <v>228</v>
+        <v>193</v>
       </c>
       <c r="H41" s="8"/>
-      <c r="J41" s="92"/>
-      <c r="K41" s="91"/>
-    </row>
-    <row r="42" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="106">
-        <v>33</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C42" s="98" t="s">
-        <v>222</v>
-      </c>
-      <c r="D42" s="104" t="s">
-        <v>216</v>
-      </c>
-      <c r="E42" s="101" t="s">
+      <c r="J41" s="62"/>
+      <c r="K41" s="61"/>
+    </row>
+    <row r="42" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="76">
+        <v>25</v>
+      </c>
+      <c r="B42" s="68" t="s">
+        <v>204</v>
+      </c>
+      <c r="C42" s="68" t="s">
+        <v>348</v>
+      </c>
+      <c r="D42" s="74" t="s">
+        <v>208</v>
+      </c>
+      <c r="E42" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F42" s="8"/>
-      <c r="G42" s="8" t="s">
-        <v>195</v>
+      <c r="G42" s="44" t="s">
+        <v>351</v>
       </c>
       <c r="H42" s="8"/>
-      <c r="J42" s="92"/>
-      <c r="K42" s="91"/>
-    </row>
-    <row r="43" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="106">
-        <v>34</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C43" s="98" t="s">
-        <v>222</v>
-      </c>
-      <c r="D43" s="104" t="s">
-        <v>217</v>
-      </c>
-      <c r="E43" s="101" t="s">
+      <c r="J42" s="62"/>
+      <c r="K42" s="61"/>
+    </row>
+    <row r="43" spans="1:11" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="76">
+        <v>26</v>
+      </c>
+      <c r="B43" s="68" t="s">
+        <v>204</v>
+      </c>
+      <c r="C43" s="68" t="s">
+        <v>349</v>
+      </c>
+      <c r="D43" s="74" t="s">
+        <v>209</v>
+      </c>
+      <c r="E43" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F43" s="8"/>
-      <c r="G43" s="30" t="s">
-        <v>229</v>
+      <c r="G43" s="44" t="s">
+        <v>350</v>
       </c>
       <c r="H43" s="8"/>
-      <c r="J43" s="92"/>
-      <c r="K43" s="91"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="61"/>
     </row>
     <row r="44" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="106">
-        <v>35</v>
+      <c r="A44" s="76">
+        <v>27</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C44" s="98" t="s">
-        <v>218</v>
-      </c>
-      <c r="D44" s="104" t="s">
-        <v>220</v>
-      </c>
-      <c r="E44" s="101" t="s">
+        <v>210</v>
+      </c>
+      <c r="C44" s="68" t="s">
+        <v>211</v>
+      </c>
+      <c r="D44" s="74" t="s">
+        <v>198</v>
+      </c>
+      <c r="E44" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="H44" s="8"/>
-      <c r="J44" s="92"/>
-      <c r="K44" s="91"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="61"/>
     </row>
     <row r="45" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="106">
-        <v>36</v>
-      </c>
-      <c r="B45" s="8" t="s">
+      <c r="A45" s="76">
+        <v>28</v>
+      </c>
+      <c r="B45" s="68" t="s">
         <v>212</v>
       </c>
-      <c r="C45" s="98" t="s">
-        <v>231</v>
-      </c>
-      <c r="D45" s="104" t="s">
-        <v>232</v>
-      </c>
-      <c r="E45" s="101" t="s">
+      <c r="C45" s="68" t="s">
+        <v>382</v>
+      </c>
+      <c r="D45" s="74" t="s">
+        <v>213</v>
+      </c>
+      <c r="E45" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="H45" s="8"/>
-      <c r="J45" s="92"/>
-      <c r="K45" s="91"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="61"/>
     </row>
     <row r="46" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="106">
-        <v>37</v>
-      </c>
-      <c r="B46" s="8" t="s">
+      <c r="A46" s="76">
+        <v>29</v>
+      </c>
+      <c r="B46" s="68" t="s">
         <v>212</v>
       </c>
-      <c r="C46" s="98" t="s">
-        <v>231</v>
-      </c>
-      <c r="D46" s="104" t="s">
-        <v>233</v>
-      </c>
-      <c r="E46" s="101" t="s">
+      <c r="C46" s="68" t="s">
+        <v>383</v>
+      </c>
+      <c r="D46" s="74" t="s">
+        <v>214</v>
+      </c>
+      <c r="E46" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H46" s="8"/>
-      <c r="J46" s="92"/>
-      <c r="K46" s="91"/>
+      <c r="J46" s="62"/>
+      <c r="K46" s="61"/>
     </row>
     <row r="47" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="106">
-        <v>38</v>
-      </c>
-      <c r="B47" s="8" t="s">
+      <c r="A47" s="76">
+        <v>30</v>
+      </c>
+      <c r="B47" s="68" t="s">
         <v>212</v>
       </c>
-      <c r="C47" s="98" t="s">
-        <v>231</v>
-      </c>
-      <c r="D47" s="104" t="s">
-        <v>234</v>
-      </c>
-      <c r="E47" s="101" t="s">
+      <c r="C47" s="68" t="s">
+        <v>384</v>
+      </c>
+      <c r="D47" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="E47" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F47" s="8"/>
-      <c r="G47" s="30" t="s">
-        <v>235</v>
+      <c r="G47" s="8" t="s">
+        <v>225</v>
       </c>
       <c r="H47" s="8"/>
-      <c r="J47" s="92"/>
-      <c r="K47" s="91"/>
+      <c r="J47" s="62"/>
+      <c r="K47" s="61"/>
     </row>
     <row r="48" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="106">
-        <v>39</v>
-      </c>
-      <c r="B48" s="8" t="s">
+      <c r="A48" s="76">
+        <v>31</v>
+      </c>
+      <c r="B48" s="68" t="s">
         <v>212</v>
       </c>
-      <c r="C48" s="98" t="s">
-        <v>237</v>
-      </c>
-      <c r="D48" s="104" t="s">
-        <v>238</v>
-      </c>
-      <c r="E48" s="101" t="s">
+      <c r="C48" s="68" t="s">
+        <v>217</v>
+      </c>
+      <c r="D48" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="E48" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="H48" s="8"/>
-      <c r="J48" s="92"/>
-      <c r="K48" s="91"/>
+      <c r="J48" s="62"/>
+      <c r="K48" s="61"/>
     </row>
     <row r="49" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="106">
-        <v>40</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C49" s="98" t="s">
-        <v>237</v>
-      </c>
-      <c r="D49" s="104" t="s">
-        <v>239</v>
-      </c>
-      <c r="E49" s="101" t="s">
+      <c r="A49" s="76">
+        <v>32</v>
+      </c>
+      <c r="B49" s="68" t="s">
+        <v>220</v>
+      </c>
+      <c r="C49" s="68" t="s">
+        <v>379</v>
+      </c>
+      <c r="D49" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="E49" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="8" t="s">
-        <v>195</v>
+        <v>226</v>
       </c>
       <c r="H49" s="8"/>
-      <c r="J49" s="92"/>
-      <c r="K49" s="91"/>
+      <c r="J49" s="62"/>
+      <c r="K49" s="61"/>
     </row>
     <row r="50" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="106">
-        <v>41</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C50" s="98" t="s">
-        <v>237</v>
-      </c>
-      <c r="D50" s="104" t="s">
-        <v>240</v>
-      </c>
-      <c r="E50" s="101" t="s">
+      <c r="A50" s="76">
+        <v>33</v>
+      </c>
+      <c r="B50" s="68" t="s">
+        <v>220</v>
+      </c>
+      <c r="C50" s="68" t="s">
+        <v>380</v>
+      </c>
+      <c r="D50" s="74" t="s">
+        <v>214</v>
+      </c>
+      <c r="E50" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F50" s="8"/>
-      <c r="G50" s="30" t="s">
-        <v>241</v>
+      <c r="G50" s="8" t="s">
+        <v>193</v>
       </c>
       <c r="H50" s="8"/>
-      <c r="J50" s="92"/>
-      <c r="K50" s="91"/>
+      <c r="J50" s="62"/>
+      <c r="K50" s="61"/>
     </row>
     <row r="51" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="106">
-        <v>42</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C51" s="98" t="s">
-        <v>243</v>
-      </c>
-      <c r="D51" s="104" t="s">
-        <v>246</v>
-      </c>
-      <c r="E51" s="101" t="s">
+      <c r="A51" s="76">
+        <v>34</v>
+      </c>
+      <c r="B51" s="68" t="s">
+        <v>220</v>
+      </c>
+      <c r="C51" s="68" t="s">
+        <v>381</v>
+      </c>
+      <c r="D51" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="E51" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F51" s="8"/>
-      <c r="G51" s="8" t="s">
-        <v>247</v>
+      <c r="G51" s="30" t="s">
+        <v>227</v>
       </c>
       <c r="H51" s="8"/>
-      <c r="J51" s="92"/>
-      <c r="K51" s="91"/>
+      <c r="J51" s="62"/>
+      <c r="K51" s="61"/>
     </row>
     <row r="52" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="106">
-        <v>43</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C52" s="98" t="s">
-        <v>243</v>
-      </c>
-      <c r="D52" s="104" t="s">
-        <v>245</v>
-      </c>
-      <c r="E52" s="101" t="s">
+      <c r="A52" s="76">
+        <v>35</v>
+      </c>
+      <c r="B52" s="68" t="s">
+        <v>220</v>
+      </c>
+      <c r="C52" s="68" t="s">
+        <v>216</v>
+      </c>
+      <c r="D52" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="E52" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F52" s="8"/>
       <c r="G52" s="8" t="s">
-        <v>195</v>
+        <v>228</v>
       </c>
       <c r="H52" s="8"/>
-      <c r="J52" s="92"/>
-      <c r="K52" s="91"/>
+      <c r="J52" s="62"/>
+      <c r="K52" s="61"/>
     </row>
     <row r="53" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="106">
-        <v>41</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C53" s="98" t="s">
-        <v>243</v>
-      </c>
-      <c r="D53" s="104" t="s">
-        <v>244</v>
-      </c>
-      <c r="E53" s="101" t="s">
+      <c r="A53" s="76">
+        <v>36</v>
+      </c>
+      <c r="B53" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="C53" s="68" t="s">
+        <v>378</v>
+      </c>
+      <c r="D53" s="74" t="s">
+        <v>230</v>
+      </c>
+      <c r="E53" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F53" s="8"/>
-      <c r="G53" s="30" t="s">
-        <v>248</v>
+      <c r="G53" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="H53" s="8"/>
-      <c r="J53" s="92"/>
-      <c r="K53" s="91"/>
+      <c r="J53" s="62"/>
+      <c r="K53" s="61"/>
     </row>
     <row r="54" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="106">
-        <v>42</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C54" s="98" t="s">
-        <v>291</v>
-      </c>
-      <c r="D54" s="104" t="s">
-        <v>292</v>
-      </c>
-      <c r="E54" s="101" t="s">
+      <c r="A54" s="76">
+        <v>37</v>
+      </c>
+      <c r="B54" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="C54" s="68" t="s">
+        <v>377</v>
+      </c>
+      <c r="D54" s="74" t="s">
+        <v>231</v>
+      </c>
+      <c r="E54" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F54" s="8"/>
       <c r="G54" s="8" t="s">
-        <v>296</v>
+        <v>193</v>
       </c>
       <c r="H54" s="8"/>
-      <c r="J54" s="92"/>
-      <c r="K54" s="91"/>
+      <c r="J54" s="62"/>
+      <c r="K54" s="61"/>
     </row>
     <row r="55" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="106">
-        <v>43</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C55" s="98" t="s">
-        <v>291</v>
-      </c>
-      <c r="D55" s="104" t="s">
-        <v>293</v>
-      </c>
-      <c r="E55" s="101" t="s">
+      <c r="A55" s="76">
+        <v>38</v>
+      </c>
+      <c r="B55" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="C55" s="68" t="s">
+        <v>376</v>
+      </c>
+      <c r="D55" s="74" t="s">
+        <v>232</v>
+      </c>
+      <c r="E55" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F55" s="8"/>
-      <c r="G55" s="8" t="s">
-        <v>195</v>
+      <c r="G55" s="30" t="s">
+        <v>233</v>
       </c>
       <c r="H55" s="8"/>
-      <c r="J55" s="92"/>
-      <c r="K55" s="91"/>
+      <c r="J55" s="62"/>
+      <c r="K55" s="61"/>
     </row>
     <row r="56" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="106">
-        <v>44</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C56" s="98" t="s">
-        <v>291</v>
-      </c>
-      <c r="D56" s="104" t="s">
-        <v>294</v>
-      </c>
-      <c r="E56" s="101" t="s">
+      <c r="A56" s="76">
+        <v>39</v>
+      </c>
+      <c r="B56" s="68" t="s">
+        <v>235</v>
+      </c>
+      <c r="C56" s="68" t="s">
+        <v>373</v>
+      </c>
+      <c r="D56" s="74" t="s">
+        <v>236</v>
+      </c>
+      <c r="E56" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F56" s="8"/>
-      <c r="G56" s="30" t="s">
-        <v>295</v>
+      <c r="G56" s="8" t="s">
+        <v>240</v>
       </c>
       <c r="H56" s="8"/>
-      <c r="J56" s="92"/>
-      <c r="K56" s="91"/>
+      <c r="J56" s="62"/>
+      <c r="K56" s="61"/>
     </row>
     <row r="57" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="106">
-        <v>45</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C57" s="98" t="s">
-        <v>249</v>
-      </c>
-      <c r="D57" s="104" t="s">
-        <v>250</v>
-      </c>
-      <c r="E57" s="101" t="s">
+      <c r="A57" s="76">
+        <v>40</v>
+      </c>
+      <c r="B57" s="68" t="s">
+        <v>235</v>
+      </c>
+      <c r="C57" s="68" t="s">
+        <v>374</v>
+      </c>
+      <c r="D57" s="74" t="s">
+        <v>237</v>
+      </c>
+      <c r="E57" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F57" s="8"/>
       <c r="G57" s="8" t="s">
-        <v>254</v>
+        <v>193</v>
       </c>
       <c r="H57" s="8"/>
-      <c r="J57" s="92"/>
-      <c r="K57" s="91"/>
+      <c r="J57" s="62"/>
+      <c r="K57" s="61"/>
     </row>
     <row r="58" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="106">
-        <v>46</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C58" s="98" t="s">
-        <v>249</v>
-      </c>
-      <c r="D58" s="104" t="s">
-        <v>251</v>
-      </c>
-      <c r="E58" s="101" t="s">
+      <c r="A58" s="76">
+        <v>41</v>
+      </c>
+      <c r="B58" s="68" t="s">
+        <v>235</v>
+      </c>
+      <c r="C58" s="68" t="s">
+        <v>375</v>
+      </c>
+      <c r="D58" s="74" t="s">
+        <v>238</v>
+      </c>
+      <c r="E58" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F58" s="8"/>
-      <c r="G58" s="8" t="s">
-        <v>195</v>
+      <c r="G58" s="30" t="s">
+        <v>239</v>
       </c>
       <c r="H58" s="8"/>
-      <c r="J58" s="92"/>
-      <c r="K58" s="91"/>
+      <c r="J58" s="62"/>
+      <c r="K58" s="61"/>
     </row>
     <row r="59" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="106">
-        <v>47</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C59" s="98" t="s">
-        <v>249</v>
-      </c>
-      <c r="D59" s="104" t="s">
-        <v>252</v>
-      </c>
-      <c r="E59" s="101" t="s">
+      <c r="A59" s="76">
+        <v>42</v>
+      </c>
+      <c r="B59" s="68" t="s">
+        <v>241</v>
+      </c>
+      <c r="C59" s="68" t="s">
+        <v>370</v>
+      </c>
+      <c r="D59" s="74" t="s">
+        <v>244</v>
+      </c>
+      <c r="E59" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F59" s="8"/>
-      <c r="G59" s="30" t="s">
-        <v>253</v>
+      <c r="G59" s="8" t="s">
+        <v>245</v>
       </c>
       <c r="H59" s="8"/>
-      <c r="J59" s="92"/>
-      <c r="K59" s="91"/>
+      <c r="J59" s="62"/>
+      <c r="K59" s="61"/>
     </row>
     <row r="60" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="106">
-        <v>48</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C60" s="98" t="s">
-        <v>257</v>
-      </c>
-      <c r="D60" s="104" t="s">
-        <v>258</v>
-      </c>
-      <c r="E60" s="101" t="s">
+      <c r="A60" s="76">
+        <v>43</v>
+      </c>
+      <c r="B60" s="68" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60" s="68" t="s">
+        <v>371</v>
+      </c>
+      <c r="D60" s="74" t="s">
+        <v>243</v>
+      </c>
+      <c r="E60" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F60" s="8"/>
       <c r="G60" s="8" t="s">
-        <v>261</v>
+        <v>193</v>
       </c>
       <c r="H60" s="8"/>
-      <c r="J60" s="92"/>
-      <c r="K60" s="91"/>
+      <c r="J60" s="62"/>
+      <c r="K60" s="61"/>
     </row>
     <row r="61" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="106">
-        <v>49</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C61" s="98" t="s">
-        <v>257</v>
-      </c>
-      <c r="D61" s="104" t="s">
-        <v>259</v>
-      </c>
-      <c r="E61" s="101" t="s">
+      <c r="A61" s="76">
+        <v>41</v>
+      </c>
+      <c r="B61" s="68" t="s">
+        <v>241</v>
+      </c>
+      <c r="C61" s="68" t="s">
+        <v>372</v>
+      </c>
+      <c r="D61" s="74" t="s">
+        <v>242</v>
+      </c>
+      <c r="E61" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F61" s="8"/>
-      <c r="G61" s="8" t="s">
-        <v>195</v>
+      <c r="G61" s="30" t="s">
+        <v>246</v>
       </c>
       <c r="H61" s="8"/>
-      <c r="J61" s="92"/>
-      <c r="K61" s="91"/>
+      <c r="J61" s="62"/>
+      <c r="K61" s="61"/>
     </row>
     <row r="62" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="106">
-        <v>50</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C62" s="98" t="s">
-        <v>257</v>
-      </c>
-      <c r="D62" s="104" t="s">
-        <v>260</v>
-      </c>
-      <c r="E62" s="101" t="s">
+      <c r="A62" s="76">
+        <v>42</v>
+      </c>
+      <c r="B62" s="68" t="s">
+        <v>287</v>
+      </c>
+      <c r="C62" s="68" t="s">
+        <v>332</v>
+      </c>
+      <c r="D62" s="74" t="s">
+        <v>288</v>
+      </c>
+      <c r="E62" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F62" s="8"/>
-      <c r="G62" s="30" t="s">
-        <v>262</v>
+      <c r="G62" s="8" t="s">
+        <v>292</v>
       </c>
       <c r="H62" s="8"/>
-      <c r="J62" s="92"/>
-      <c r="K62" s="91"/>
+      <c r="J62" s="62"/>
+      <c r="K62" s="61"/>
     </row>
     <row r="63" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="106">
-        <v>51</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C63" s="98" t="s">
-        <v>257</v>
-      </c>
-      <c r="D63" s="104" t="s">
-        <v>263</v>
-      </c>
-      <c r="E63" s="101" t="s">
+      <c r="A63" s="76">
+        <v>43</v>
+      </c>
+      <c r="B63" s="68" t="s">
+        <v>287</v>
+      </c>
+      <c r="C63" s="68" t="s">
+        <v>333</v>
+      </c>
+      <c r="D63" s="74" t="s">
+        <v>289</v>
+      </c>
+      <c r="E63" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F63" s="8"/>
       <c r="G63" s="8" t="s">
-        <v>264</v>
+        <v>193</v>
       </c>
       <c r="H63" s="8"/>
-      <c r="J63" s="92"/>
-      <c r="K63" s="91"/>
+      <c r="J63" s="62"/>
+      <c r="K63" s="61"/>
     </row>
     <row r="64" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="106">
-        <v>52</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C64" s="98" t="s">
-        <v>265</v>
-      </c>
-      <c r="D64" s="104" t="s">
-        <v>266</v>
-      </c>
-      <c r="E64" s="101" t="s">
+      <c r="A64" s="76">
+        <v>44</v>
+      </c>
+      <c r="B64" s="68" t="s">
+        <v>287</v>
+      </c>
+      <c r="C64" s="68" t="s">
+        <v>334</v>
+      </c>
+      <c r="D64" s="74" t="s">
+        <v>290</v>
+      </c>
+      <c r="E64" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F64" s="8"/>
-      <c r="G64" s="8" t="s">
-        <v>271</v>
+      <c r="G64" s="30" t="s">
+        <v>291</v>
       </c>
       <c r="H64" s="8"/>
-      <c r="J64" s="92"/>
-      <c r="K64" s="91"/>
+      <c r="J64" s="62"/>
+      <c r="K64" s="61"/>
     </row>
     <row r="65" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="106">
-        <v>53</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C65" s="98" t="s">
-        <v>265</v>
-      </c>
-      <c r="D65" s="104" t="s">
-        <v>267</v>
-      </c>
-      <c r="E65" s="101" t="s">
+      <c r="A65" s="76">
+        <v>45</v>
+      </c>
+      <c r="B65" s="68" t="s">
+        <v>247</v>
+      </c>
+      <c r="C65" s="68" t="s">
+        <v>335</v>
+      </c>
+      <c r="D65" s="74" t="s">
+        <v>248</v>
+      </c>
+      <c r="E65" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F65" s="8"/>
       <c r="G65" s="8" t="s">
-        <v>195</v>
+        <v>252</v>
       </c>
       <c r="H65" s="8"/>
-      <c r="J65" s="92"/>
-      <c r="K65" s="91"/>
+      <c r="J65" s="62"/>
+      <c r="K65" s="61"/>
     </row>
     <row r="66" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="106">
-        <v>54</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C66" s="98" t="s">
-        <v>265</v>
-      </c>
-      <c r="D66" s="104" t="s">
-        <v>268</v>
-      </c>
-      <c r="E66" s="101" t="s">
+      <c r="A66" s="76">
+        <v>46</v>
+      </c>
+      <c r="B66" s="68" t="s">
+        <v>247</v>
+      </c>
+      <c r="C66" s="68" t="s">
+        <v>336</v>
+      </c>
+      <c r="D66" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="E66" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F66" s="8"/>
-      <c r="G66" s="30" t="s">
-        <v>270</v>
+      <c r="G66" s="8" t="s">
+        <v>193</v>
       </c>
       <c r="H66" s="8"/>
-      <c r="J66" s="92"/>
-      <c r="K66" s="91"/>
+      <c r="J66" s="62"/>
+      <c r="K66" s="61"/>
     </row>
     <row r="67" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="106">
-        <v>55</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C67" s="98" t="s">
-        <v>265</v>
-      </c>
-      <c r="D67" s="104" t="s">
-        <v>269</v>
-      </c>
-      <c r="E67" s="101" t="s">
+      <c r="A67" s="76">
+        <v>47</v>
+      </c>
+      <c r="B67" s="68" t="s">
+        <v>247</v>
+      </c>
+      <c r="C67" s="68" t="s">
+        <v>337</v>
+      </c>
+      <c r="D67" s="74" t="s">
+        <v>250</v>
+      </c>
+      <c r="E67" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F67" s="8"/>
-      <c r="G67" s="8" t="s">
-        <v>264</v>
+      <c r="G67" s="30" t="s">
+        <v>251</v>
       </c>
       <c r="H67" s="8"/>
-      <c r="J67" s="92"/>
-      <c r="K67" s="91"/>
+      <c r="J67" s="62"/>
+      <c r="K67" s="61"/>
     </row>
     <row r="68" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="106">
-        <v>56</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C68" s="98" t="s">
-        <v>272</v>
-      </c>
-      <c r="D68" s="98" t="s">
-        <v>272</v>
-      </c>
-      <c r="E68" s="101" t="s">
+      <c r="A68" s="76">
+        <v>48</v>
+      </c>
+      <c r="B68" s="68" t="s">
+        <v>253</v>
+      </c>
+      <c r="C68" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="D68" s="74" t="s">
+        <v>254</v>
+      </c>
+      <c r="E68" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F68" s="8"/>
       <c r="G68" s="8" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="H68" s="8"/>
-      <c r="J68" s="92"/>
-      <c r="K68" s="91"/>
+      <c r="J68" s="62"/>
+      <c r="K68" s="61"/>
     </row>
     <row r="69" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="106">
-        <v>57</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C69" s="98" t="s">
-        <v>274</v>
-      </c>
-      <c r="D69" s="98" t="s">
-        <v>274</v>
-      </c>
-      <c r="E69" s="101" t="s">
+      <c r="A69" s="76">
+        <v>49</v>
+      </c>
+      <c r="B69" s="68" t="s">
+        <v>253</v>
+      </c>
+      <c r="C69" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="D69" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="E69" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F69" s="8"/>
       <c r="G69" s="8" t="s">
-        <v>275</v>
+        <v>193</v>
       </c>
       <c r="H69" s="8"/>
-      <c r="J69" s="92"/>
-      <c r="K69" s="91"/>
+      <c r="J69" s="62"/>
+      <c r="K69" s="61"/>
     </row>
     <row r="70" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="106">
-        <v>58</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C70" s="98" t="s">
-        <v>277</v>
-      </c>
-      <c r="D70" s="104" t="s">
-        <v>278</v>
-      </c>
-      <c r="E70" s="101" t="s">
+      <c r="A70" s="76">
+        <v>50</v>
+      </c>
+      <c r="B70" s="68" t="s">
+        <v>253</v>
+      </c>
+      <c r="C70" s="68" t="s">
+        <v>340</v>
+      </c>
+      <c r="D70" s="74" t="s">
+        <v>256</v>
+      </c>
+      <c r="E70" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F70" s="8"/>
-      <c r="G70" s="8" t="s">
-        <v>279</v>
+      <c r="G70" s="30" t="s">
+        <v>258</v>
       </c>
       <c r="H70" s="8"/>
-      <c r="J70" s="92"/>
-      <c r="K70" s="91"/>
+      <c r="J70" s="62"/>
+      <c r="K70" s="61"/>
     </row>
     <row r="71" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="106">
-        <v>59</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C71" s="98" t="s">
-        <v>280</v>
-      </c>
-      <c r="D71" s="104" t="s">
-        <v>278</v>
-      </c>
-      <c r="E71" s="101" t="s">
+      <c r="A71" s="76">
+        <v>51</v>
+      </c>
+      <c r="B71" s="68" t="s">
+        <v>253</v>
+      </c>
+      <c r="C71" s="68" t="s">
+        <v>341</v>
+      </c>
+      <c r="D71" s="74" t="s">
+        <v>259</v>
+      </c>
+      <c r="E71" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F71" s="8"/>
       <c r="G71" s="8" t="s">
-        <v>299</v>
+        <v>260</v>
       </c>
       <c r="H71" s="8"/>
-      <c r="J71" s="92"/>
-      <c r="K71" s="91"/>
+      <c r="J71" s="62"/>
+      <c r="K71" s="61"/>
     </row>
     <row r="72" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="106">
-        <v>60</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C72" s="98" t="s">
-        <v>281</v>
-      </c>
-      <c r="D72" s="104" t="s">
-        <v>278</v>
-      </c>
-      <c r="E72" s="101" t="s">
+      <c r="A72" s="76">
+        <v>52</v>
+      </c>
+      <c r="B72" s="68" t="s">
+        <v>261</v>
+      </c>
+      <c r="C72" s="68" t="s">
+        <v>342</v>
+      </c>
+      <c r="D72" s="74" t="s">
+        <v>262</v>
+      </c>
+      <c r="E72" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F72" s="8"/>
       <c r="G72" s="8" t="s">
-        <v>301</v>
+        <v>267</v>
       </c>
       <c r="H72" s="8"/>
-      <c r="J72" s="92"/>
-      <c r="K72" s="91"/>
+      <c r="J72" s="62"/>
+      <c r="K72" s="61"/>
     </row>
     <row r="73" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="106">
-        <v>61</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C73" s="98" t="s">
-        <v>282</v>
-      </c>
-      <c r="D73" s="104" t="s">
-        <v>278</v>
-      </c>
-      <c r="E73" s="101" t="s">
+      <c r="A73" s="76">
+        <v>53</v>
+      </c>
+      <c r="B73" s="68" t="s">
+        <v>261</v>
+      </c>
+      <c r="C73" s="68" t="s">
+        <v>343</v>
+      </c>
+      <c r="D73" s="74" t="s">
+        <v>263</v>
+      </c>
+      <c r="E73" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F73" s="8"/>
       <c r="G73" s="8" t="s">
-        <v>300</v>
+        <v>193</v>
       </c>
       <c r="H73" s="8"/>
-      <c r="J73" s="92"/>
-      <c r="K73" s="91"/>
+      <c r="J73" s="62"/>
+      <c r="K73" s="61"/>
     </row>
     <row r="74" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="106">
-        <v>62</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C74" s="98" t="s">
-        <v>283</v>
-      </c>
-      <c r="D74" s="104" t="s">
-        <v>278</v>
-      </c>
-      <c r="E74" s="101" t="s">
+      <c r="A74" s="76">
+        <v>54</v>
+      </c>
+      <c r="B74" s="68" t="s">
+        <v>261</v>
+      </c>
+      <c r="C74" s="68" t="s">
+        <v>344</v>
+      </c>
+      <c r="D74" s="74" t="s">
+        <v>264</v>
+      </c>
+      <c r="E74" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F74" s="8"/>
-      <c r="G74" s="8" t="s">
-        <v>302</v>
+      <c r="G74" s="30" t="s">
+        <v>266</v>
       </c>
       <c r="H74" s="8"/>
-      <c r="J74" s="92"/>
-      <c r="K74" s="91"/>
+      <c r="J74" s="62"/>
+      <c r="K74" s="61"/>
     </row>
     <row r="75" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="106">
-        <v>63</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C75" s="98" t="s">
-        <v>284</v>
-      </c>
-      <c r="D75" s="104" t="s">
-        <v>278</v>
-      </c>
-      <c r="E75" s="101" t="s">
+      <c r="A75" s="76">
+        <v>55</v>
+      </c>
+      <c r="B75" s="68" t="s">
+        <v>261</v>
+      </c>
+      <c r="C75" s="68" t="s">
+        <v>345</v>
+      </c>
+      <c r="D75" s="74" t="s">
+        <v>265</v>
+      </c>
+      <c r="E75" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F75" s="8"/>
       <c r="G75" s="8" t="s">
-        <v>298</v>
+        <v>260</v>
       </c>
       <c r="H75" s="8"/>
-      <c r="J75" s="92"/>
-      <c r="K75" s="91"/>
+      <c r="J75" s="62"/>
+      <c r="K75" s="61"/>
     </row>
     <row r="76" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="106">
-        <v>64</v>
+      <c r="A76" s="76">
+        <v>56</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C76" s="98" t="s">
-        <v>285</v>
-      </c>
-      <c r="D76" s="104" t="s">
-        <v>278</v>
-      </c>
-      <c r="E76" s="101" t="s">
+        <v>210</v>
+      </c>
+      <c r="C76" s="68" t="s">
+        <v>268</v>
+      </c>
+      <c r="D76" s="68" t="s">
+        <v>268</v>
+      </c>
+      <c r="E76" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F76" s="8"/>
       <c r="G76" s="8" t="s">
-        <v>303</v>
+        <v>269</v>
       </c>
       <c r="H76" s="8"/>
-      <c r="J76" s="92"/>
-      <c r="K76" s="91"/>
+      <c r="J76" s="62"/>
+      <c r="K76" s="61"/>
     </row>
     <row r="77" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="106">
-        <v>65</v>
+      <c r="A77" s="76">
+        <v>57</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C77" s="98" t="s">
-        <v>286</v>
-      </c>
-      <c r="D77" s="104" t="s">
-        <v>278</v>
-      </c>
-      <c r="E77" s="101" t="s">
+        <v>210</v>
+      </c>
+      <c r="C77" s="68" t="s">
+        <v>270</v>
+      </c>
+      <c r="D77" s="68" t="s">
+        <v>270</v>
+      </c>
+      <c r="E77" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F77" s="8"/>
       <c r="G77" s="8" t="s">
-        <v>304</v>
+        <v>271</v>
       </c>
       <c r="H77" s="8"/>
-      <c r="J77" s="92"/>
-      <c r="K77" s="91"/>
+      <c r="J77" s="62"/>
+      <c r="K77" s="61"/>
     </row>
     <row r="78" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="106">
-        <v>66</v>
+      <c r="A78" s="76">
+        <v>58</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C78" s="98" t="s">
-        <v>287</v>
-      </c>
-      <c r="D78" s="104" t="s">
-        <v>278</v>
-      </c>
-      <c r="E78" s="101" t="s">
+        <v>272</v>
+      </c>
+      <c r="C78" s="68" t="s">
+        <v>273</v>
+      </c>
+      <c r="D78" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="E78" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F78" s="8"/>
       <c r="G78" s="8" t="s">
-        <v>305</v>
+        <v>275</v>
       </c>
       <c r="H78" s="8"/>
-      <c r="J78" s="92"/>
-      <c r="K78" s="91"/>
+      <c r="J78" s="62"/>
+      <c r="K78" s="61"/>
     </row>
     <row r="79" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="106">
-        <v>67</v>
+      <c r="A79" s="76">
+        <v>59</v>
       </c>
       <c r="B79" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C79" s="68" t="s">
         <v>276</v>
       </c>
-      <c r="C79" s="98" t="s">
-        <v>288</v>
-      </c>
-      <c r="D79" s="104" t="s">
-        <v>278</v>
-      </c>
-      <c r="E79" s="101" t="s">
+      <c r="D79" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="E79" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F79" s="8"/>
       <c r="G79" s="8" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="H79" s="8"/>
-      <c r="J79" s="92"/>
-      <c r="K79" s="91"/>
+      <c r="J79" s="62"/>
+      <c r="K79" s="61"/>
     </row>
     <row r="80" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="106">
-        <v>68</v>
+      <c r="A80" s="76">
+        <v>60</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C80" s="98" t="s">
-        <v>289</v>
-      </c>
-      <c r="D80" s="104" t="s">
-        <v>278</v>
-      </c>
-      <c r="E80" s="101" t="s">
+        <v>272</v>
+      </c>
+      <c r="C80" s="68" t="s">
+        <v>277</v>
+      </c>
+      <c r="D80" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="E80" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F80" s="8"/>
       <c r="G80" s="8" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="H80" s="8"/>
-      <c r="J80" s="92"/>
-      <c r="K80" s="91"/>
+      <c r="J80" s="62"/>
+      <c r="K80" s="61"/>
     </row>
     <row r="81" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="106">
-        <v>69</v>
+      <c r="A81" s="76">
+        <v>61</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C81" s="98" t="s">
-        <v>290</v>
-      </c>
-      <c r="D81" s="104" t="s">
+        <v>272</v>
+      </c>
+      <c r="C81" s="68" t="s">
         <v>278</v>
       </c>
-      <c r="E81" s="101" t="s">
+      <c r="D81" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="E81" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F81" s="8"/>
       <c r="G81" s="8" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="H81" s="8"/>
-      <c r="J81" s="92"/>
-      <c r="K81" s="91"/>
+      <c r="J81" s="62"/>
+      <c r="K81" s="61"/>
     </row>
     <row r="82" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="106">
-        <v>70</v>
+      <c r="A82" s="76">
+        <v>62</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C82" s="98" t="s">
-        <v>297</v>
-      </c>
-      <c r="D82" s="104" t="s">
-        <v>278</v>
-      </c>
-      <c r="E82" s="101" t="s">
+        <v>272</v>
+      </c>
+      <c r="C82" s="68" t="s">
+        <v>279</v>
+      </c>
+      <c r="D82" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="E82" s="71" t="s">
         <v>72</v>
       </c>
       <c r="F82" s="8"/>
       <c r="G82" s="8" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="H82" s="8"/>
-      <c r="J82" s="92"/>
-      <c r="K82" s="91"/>
+      <c r="J82" s="62"/>
+      <c r="K82" s="61"/>
     </row>
     <row r="83" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="6">
-        <v>71</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C83" s="95" t="s">
-        <v>316</v>
-      </c>
-      <c r="D83" s="95" t="s">
-        <v>318</v>
-      </c>
-      <c r="E83" s="101" t="s">
-        <v>46</v>
+      <c r="A83" s="76">
+        <v>63</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C83" s="68" t="s">
+        <v>280</v>
+      </c>
+      <c r="D83" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="E83" s="71" t="s">
+        <v>72</v>
       </c>
       <c r="F83" s="8"/>
       <c r="G83" s="8" t="s">
-        <v>320</v>
+        <v>294</v>
       </c>
       <c r="H83" s="8"/>
-      <c r="J83" s="7"/>
-      <c r="K83" s="8"/>
+      <c r="J83" s="62"/>
+      <c r="K83" s="61"/>
     </row>
     <row r="84" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="6">
-        <v>72</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C84" s="95" t="s">
-        <v>317</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="E84" s="101" t="s">
-        <v>99</v>
+      <c r="A84" s="76">
+        <v>64</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C84" s="68" t="s">
+        <v>281</v>
+      </c>
+      <c r="D84" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="E84" s="71" t="s">
+        <v>72</v>
       </c>
       <c r="F84" s="8"/>
       <c r="G84" s="8" t="s">
-        <v>321</v>
+        <v>299</v>
       </c>
       <c r="H84" s="8"/>
-      <c r="J84" s="7"/>
-      <c r="K84" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" s="4" customFormat="1" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="16">
-        <v>73</v>
-      </c>
-      <c r="B85" s="98" t="s">
-        <v>322</v>
-      </c>
-      <c r="C85" s="98" t="s">
-        <v>323</v>
-      </c>
-      <c r="D85" s="98" t="s">
-        <v>324</v>
-      </c>
-      <c r="E85" s="101"/>
+      <c r="J84" s="62"/>
+      <c r="K84" s="61"/>
+    </row>
+    <row r="85" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="76">
+        <v>65</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C85" s="68" t="s">
+        <v>282</v>
+      </c>
+      <c r="D85" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="E85" s="71" t="s">
+        <v>72</v>
+      </c>
       <c r="F85" s="8"/>
       <c r="G85" s="8" t="s">
-        <v>325</v>
+        <v>300</v>
       </c>
       <c r="H85" s="8"/>
-      <c r="I85"/>
-      <c r="J85" s="8"/>
-      <c r="K85" s="8"/>
-    </row>
-    <row r="86" spans="1:11" s="4" customFormat="1" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="16">
+      <c r="J85" s="62"/>
+      <c r="K85" s="61"/>
+    </row>
+    <row r="86" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="76">
+        <v>66</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C86" s="68" t="s">
+        <v>283</v>
+      </c>
+      <c r="D86" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="E86" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="H86" s="8"/>
+      <c r="J86" s="62"/>
+      <c r="K86" s="61"/>
+    </row>
+    <row r="87" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="76">
+        <v>67</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C87" s="68" t="s">
+        <v>284</v>
+      </c>
+      <c r="D87" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="E87" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="F87" s="8"/>
+      <c r="G87" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="H87" s="8"/>
+      <c r="J87" s="62"/>
+      <c r="K87" s="61"/>
+    </row>
+    <row r="88" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="76">
+        <v>68</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C88" s="68" t="s">
+        <v>285</v>
+      </c>
+      <c r="D88" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="E88" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H88" s="8"/>
+      <c r="J88" s="62"/>
+      <c r="K88" s="61"/>
+    </row>
+    <row r="89" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="76">
+        <v>69</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C89" s="68" t="s">
+        <v>286</v>
+      </c>
+      <c r="D89" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="E89" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="H89" s="8"/>
+      <c r="J89" s="62"/>
+      <c r="K89" s="61"/>
+    </row>
+    <row r="90" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="76">
+        <v>70</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C90" s="68" t="s">
+        <v>293</v>
+      </c>
+      <c r="D90" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="E90" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="F90" s="8"/>
+      <c r="G90" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="H90" s="8"/>
+      <c r="J90" s="62"/>
+      <c r="K90" s="61"/>
+    </row>
+    <row r="91" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="6">
+        <v>71</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C91" s="65" t="s">
+        <v>311</v>
+      </c>
+      <c r="D91" s="65" t="s">
+        <v>313</v>
+      </c>
+      <c r="E91" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="F91" s="8"/>
+      <c r="G91" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="H91" s="8"/>
+      <c r="J91" s="7"/>
+      <c r="K91" s="8"/>
+    </row>
+    <row r="92" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="6">
+        <v>72</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C92" s="65" t="s">
+        <v>312</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="E92" s="71" t="s">
+        <v>99</v>
+      </c>
+      <c r="F92" s="8"/>
+      <c r="G92" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="H92" s="8"/>
+      <c r="J92" s="7"/>
+      <c r="K92"/>
+    </row>
+    <row r="93" spans="1:11" s="4" customFormat="1" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="16">
+        <v>73</v>
+      </c>
+      <c r="B93" s="68" t="s">
+        <v>317</v>
+      </c>
+      <c r="C93" s="68" t="s">
+        <v>318</v>
+      </c>
+      <c r="D93" s="68" t="s">
+        <v>319</v>
+      </c>
+      <c r="E93" s="71" t="s">
+        <v>331</v>
+      </c>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="H93" s="8"/>
+      <c r="I93"/>
+      <c r="J93" s="8"/>
+      <c r="K93" s="8"/>
+    </row>
+    <row r="94" spans="1:11" s="4" customFormat="1" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="16">
         <v>74</v>
       </c>
-      <c r="B86" s="98" t="s">
+      <c r="B94" s="68" t="s">
+        <v>317</v>
+      </c>
+      <c r="C94" s="67" t="s">
+        <v>321</v>
+      </c>
+      <c r="D94" s="17"/>
+      <c r="E94" s="71" t="s">
+        <v>331</v>
+      </c>
+      <c r="F94" s="17"/>
+      <c r="G94" s="17" t="s">
         <v>322</v>
       </c>
-      <c r="C86" s="97" t="s">
-        <v>326</v>
-      </c>
-      <c r="D86" s="17"/>
-      <c r="E86" s="103"/>
-      <c r="F86" s="17"/>
-      <c r="G86" s="17" t="s">
-        <v>327</v>
-      </c>
-      <c r="H86" s="17"/>
-      <c r="I86"/>
-      <c r="J86" s="17"/>
-      <c r="K86" s="17"/>
-    </row>
-    <row r="87" spans="1:11" s="4" customFormat="1" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="16">
-        <v>75</v>
-      </c>
-      <c r="B87" s="98" t="s">
-        <v>322</v>
-      </c>
-      <c r="C87" s="97" t="s">
-        <v>328</v>
-      </c>
-      <c r="D87" s="17"/>
-      <c r="E87" s="103"/>
-      <c r="F87" s="17"/>
-      <c r="G87" s="17" t="s">
-        <v>329</v>
-      </c>
-      <c r="H87" s="17"/>
-      <c r="I87"/>
-      <c r="J87" s="17"/>
-      <c r="K87" s="17"/>
-    </row>
-    <row r="88" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="16"/>
-      <c r="B88" s="17"/>
-      <c r="C88" s="97"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="103"/>
-      <c r="F88" s="17"/>
-      <c r="G88" s="17"/>
-      <c r="H88" s="17"/>
-      <c r="I88"/>
-      <c r="J88" s="17"/>
-      <c r="K88" s="17"/>
-    </row>
-    <row r="89" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="16"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="97"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="103"/>
-      <c r="F89" s="17"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
-      <c r="I89"/>
-      <c r="J89" s="17"/>
-      <c r="K89" s="17"/>
-    </row>
-    <row r="90" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="16"/>
-      <c r="B90" s="17"/>
-      <c r="C90" s="97"/>
-      <c r="D90" s="17"/>
-      <c r="E90" s="103"/>
-      <c r="F90" s="17"/>
-      <c r="G90" s="17"/>
-      <c r="H90" s="17"/>
-      <c r="I90"/>
-      <c r="J90" s="17"/>
-      <c r="K90" s="17"/>
-    </row>
-    <row r="91" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="16"/>
-      <c r="B91" s="17"/>
-      <c r="C91" s="97"/>
-      <c r="D91" s="17"/>
-      <c r="E91" s="103"/>
-      <c r="F91" s="17"/>
-      <c r="G91" s="17"/>
-      <c r="H91" s="17"/>
-      <c r="I91"/>
-      <c r="J91" s="17"/>
-      <c r="K91" s="17"/>
-    </row>
-    <row r="92" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="16"/>
-      <c r="B92" s="17"/>
-      <c r="C92" s="97"/>
-      <c r="D92" s="17"/>
-      <c r="E92" s="103"/>
-      <c r="F92" s="17"/>
-      <c r="G92" s="17"/>
-      <c r="H92" s="17"/>
-      <c r="I92"/>
-      <c r="J92" s="17"/>
-      <c r="K92" s="17"/>
-    </row>
-    <row r="93" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="16"/>
-      <c r="B93" s="17"/>
-      <c r="C93" s="97"/>
-      <c r="D93" s="17"/>
-      <c r="E93" s="103"/>
-      <c r="F93" s="17"/>
-      <c r="G93" s="17"/>
-      <c r="H93" s="17"/>
-      <c r="I93"/>
-      <c r="J93" s="17"/>
-      <c r="K93" s="17"/>
-    </row>
-    <row r="94" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="16"/>
-      <c r="B94" s="17"/>
-      <c r="C94" s="97"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="103"/>
-      <c r="F94" s="17"/>
-      <c r="G94" s="17"/>
       <c r="H94" s="17"/>
       <c r="I94"/>
       <c r="J94" s="17"/>
       <c r="K94" s="17"/>
     </row>
-    <row r="95" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="16"/>
-      <c r="B95" s="17"/>
-      <c r="C95" s="97"/>
+    <row r="95" spans="1:11" s="4" customFormat="1" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="16">
+        <v>75</v>
+      </c>
+      <c r="B95" s="68" t="s">
+        <v>317</v>
+      </c>
+      <c r="C95" s="67" t="s">
+        <v>323</v>
+      </c>
       <c r="D95" s="17"/>
-      <c r="E95" s="103"/>
+      <c r="E95" s="71" t="s">
+        <v>331</v>
+      </c>
       <c r="F95" s="17"/>
-      <c r="G95" s="17"/>
+      <c r="G95" s="17" t="s">
+        <v>324</v>
+      </c>
       <c r="H95" s="17"/>
       <c r="I95"/>
       <c r="J95" s="17"/>
@@ -4234,9 +4491,9 @@
     <row r="96" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="16"/>
       <c r="B96" s="17"/>
-      <c r="C96" s="97"/>
+      <c r="C96" s="67"/>
       <c r="D96" s="17"/>
-      <c r="E96" s="103"/>
+      <c r="E96" s="73"/>
       <c r="F96" s="17"/>
       <c r="G96" s="17"/>
       <c r="H96" s="17"/>
@@ -4246,23 +4503,23 @@
     </row>
     <row r="97" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="16"/>
-      <c r="B97" s="8"/>
-      <c r="C97" s="98"/>
-      <c r="D97" s="8"/>
-      <c r="E97" s="101"/>
-      <c r="F97" s="8"/>
-      <c r="G97" s="8"/>
-      <c r="H97" s="8"/>
+      <c r="B97" s="17"/>
+      <c r="C97" s="67"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="73"/>
+      <c r="F97" s="17"/>
+      <c r="G97" s="17"/>
+      <c r="H97" s="17"/>
       <c r="I97"/>
-      <c r="J97" s="8"/>
-      <c r="K97" s="8"/>
+      <c r="J97" s="17"/>
+      <c r="K97" s="17"/>
     </row>
     <row r="98" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="16"/>
       <c r="B98" s="17"/>
-      <c r="C98" s="97"/>
+      <c r="C98" s="67"/>
       <c r="D98" s="17"/>
-      <c r="E98" s="103"/>
+      <c r="E98" s="73"/>
       <c r="F98" s="17"/>
       <c r="G98" s="17"/>
       <c r="H98" s="17"/>
@@ -4273,9 +4530,9 @@
     <row r="99" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="16"/>
       <c r="B99" s="17"/>
-      <c r="C99" s="97"/>
+      <c r="C99" s="67"/>
       <c r="D99" s="17"/>
-      <c r="E99" s="103"/>
+      <c r="E99" s="73"/>
       <c r="F99" s="17"/>
       <c r="G99" s="17"/>
       <c r="H99" s="17"/>
@@ -4286,9 +4543,9 @@
     <row r="100" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="16"/>
       <c r="B100" s="17"/>
-      <c r="C100" s="97"/>
+      <c r="C100" s="67"/>
       <c r="D100" s="17"/>
-      <c r="E100" s="103"/>
+      <c r="E100" s="73"/>
       <c r="F100" s="17"/>
       <c r="G100" s="17"/>
       <c r="H100" s="17"/>
@@ -4299,9 +4556,9 @@
     <row r="101" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="16"/>
       <c r="B101" s="17"/>
-      <c r="C101" s="97"/>
+      <c r="C101" s="67"/>
       <c r="D101" s="17"/>
-      <c r="E101" s="103"/>
+      <c r="E101" s="73"/>
       <c r="F101" s="17"/>
       <c r="G101" s="17"/>
       <c r="H101" s="17"/>
@@ -4312,9 +4569,9 @@
     <row r="102" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="16"/>
       <c r="B102" s="17"/>
-      <c r="C102" s="97"/>
+      <c r="C102" s="67"/>
       <c r="D102" s="17"/>
-      <c r="E102" s="103"/>
+      <c r="E102" s="73"/>
       <c r="F102" s="17"/>
       <c r="G102" s="17"/>
       <c r="H102" s="17"/>
@@ -4325,9 +4582,9 @@
     <row r="103" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="16"/>
       <c r="B103" s="17"/>
-      <c r="C103" s="97"/>
+      <c r="C103" s="67"/>
       <c r="D103" s="17"/>
-      <c r="E103" s="103"/>
+      <c r="E103" s="73"/>
       <c r="F103" s="17"/>
       <c r="G103" s="17"/>
       <c r="H103" s="17"/>
@@ -4338,9 +4595,9 @@
     <row r="104" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="16"/>
       <c r="B104" s="17"/>
-      <c r="C104" s="97"/>
+      <c r="C104" s="67"/>
       <c r="D104" s="17"/>
-      <c r="E104" s="103"/>
+      <c r="E104" s="73"/>
       <c r="F104" s="17"/>
       <c r="G104" s="17"/>
       <c r="H104" s="17"/>
@@ -4350,23 +4607,23 @@
     </row>
     <row r="105" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="16"/>
-      <c r="B105" s="17"/>
-      <c r="C105" s="97"/>
-      <c r="D105" s="17"/>
-      <c r="E105" s="103"/>
-      <c r="F105" s="17"/>
-      <c r="G105" s="17"/>
-      <c r="H105" s="17"/>
+      <c r="B105" s="8"/>
+      <c r="C105" s="68"/>
+      <c r="D105" s="8"/>
+      <c r="E105" s="71"/>
+      <c r="F105" s="8"/>
+      <c r="G105" s="8"/>
+      <c r="H105" s="8"/>
       <c r="I105"/>
-      <c r="J105" s="17"/>
-      <c r="K105" s="17"/>
+      <c r="J105" s="8"/>
+      <c r="K105" s="8"/>
     </row>
     <row r="106" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="16"/>
       <c r="B106" s="17"/>
-      <c r="C106" s="97"/>
+      <c r="C106" s="67"/>
       <c r="D106" s="17"/>
-      <c r="E106" s="103"/>
+      <c r="E106" s="73"/>
       <c r="F106" s="17"/>
       <c r="G106" s="17"/>
       <c r="H106" s="17"/>
@@ -4377,9 +4634,9 @@
     <row r="107" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="16"/>
       <c r="B107" s="17"/>
-      <c r="C107" s="97"/>
+      <c r="C107" s="67"/>
       <c r="D107" s="17"/>
-      <c r="E107" s="103"/>
+      <c r="E107" s="73"/>
       <c r="F107" s="17"/>
       <c r="G107" s="17"/>
       <c r="H107" s="17"/>
@@ -4390,9 +4647,9 @@
     <row r="108" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="16"/>
       <c r="B108" s="17"/>
-      <c r="C108" s="97"/>
+      <c r="C108" s="67"/>
       <c r="D108" s="17"/>
-      <c r="E108" s="103"/>
+      <c r="E108" s="73"/>
       <c r="F108" s="17"/>
       <c r="G108" s="17"/>
       <c r="H108" s="17"/>
@@ -4403,9 +4660,9 @@
     <row r="109" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="16"/>
       <c r="B109" s="17"/>
-      <c r="C109" s="97"/>
+      <c r="C109" s="67"/>
       <c r="D109" s="17"/>
-      <c r="E109" s="103"/>
+      <c r="E109" s="73"/>
       <c r="F109" s="17"/>
       <c r="G109" s="17"/>
       <c r="H109" s="17"/>
@@ -4416,9 +4673,9 @@
     <row r="110" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="16"/>
       <c r="B110" s="17"/>
-      <c r="C110" s="97"/>
+      <c r="C110" s="67"/>
       <c r="D110" s="17"/>
-      <c r="E110" s="103"/>
+      <c r="E110" s="73"/>
       <c r="F110" s="17"/>
       <c r="G110" s="17"/>
       <c r="H110" s="17"/>
@@ -4429,9 +4686,9 @@
     <row r="111" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="16"/>
       <c r="B111" s="17"/>
-      <c r="C111" s="97"/>
+      <c r="C111" s="67"/>
       <c r="D111" s="17"/>
-      <c r="E111" s="103"/>
+      <c r="E111" s="73"/>
       <c r="F111" s="17"/>
       <c r="G111" s="17"/>
       <c r="H111" s="17"/>
@@ -4441,114 +4698,114 @@
     </row>
     <row r="112" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="16"/>
-      <c r="B112" s="8"/>
-      <c r="C112" s="98"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="101"/>
-      <c r="F112" s="8"/>
-      <c r="G112" s="8"/>
-      <c r="H112" s="8"/>
+      <c r="B112" s="17"/>
+      <c r="C112" s="67"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="73"/>
+      <c r="F112" s="17"/>
+      <c r="G112" s="17"/>
+      <c r="H112" s="17"/>
       <c r="I112"/>
-      <c r="J112" s="8"/>
-      <c r="K112" s="8"/>
+      <c r="J112" s="17"/>
+      <c r="K112" s="17"/>
     </row>
     <row r="113" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="16"/>
-      <c r="B113" s="8"/>
-      <c r="C113" s="98"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="101"/>
-      <c r="F113" s="8"/>
-      <c r="G113" s="8"/>
-      <c r="H113" s="8"/>
+      <c r="B113" s="17"/>
+      <c r="C113" s="67"/>
+      <c r="D113" s="17"/>
+      <c r="E113" s="73"/>
+      <c r="F113" s="17"/>
+      <c r="G113" s="17"/>
+      <c r="H113" s="17"/>
       <c r="I113"/>
-      <c r="J113" s="8"/>
-      <c r="K113" s="8"/>
+      <c r="J113" s="17"/>
+      <c r="K113" s="17"/>
     </row>
     <row r="114" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="16"/>
-      <c r="B114" s="8"/>
-      <c r="C114" s="98"/>
-      <c r="D114" s="8"/>
-      <c r="E114" s="101"/>
-      <c r="F114" s="8"/>
-      <c r="G114" s="8"/>
-      <c r="H114" s="8"/>
+      <c r="B114" s="17"/>
+      <c r="C114" s="67"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="73"/>
+      <c r="F114" s="17"/>
+      <c r="G114" s="17"/>
+      <c r="H114" s="17"/>
       <c r="I114"/>
-      <c r="J114" s="8"/>
-      <c r="K114" s="8"/>
+      <c r="J114" s="17"/>
+      <c r="K114" s="17"/>
     </row>
     <row r="115" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="16"/>
-      <c r="B115" s="8"/>
-      <c r="C115" s="98"/>
-      <c r="D115" s="8"/>
-      <c r="E115" s="101"/>
-      <c r="F115" s="8"/>
-      <c r="G115" s="8"/>
-      <c r="H115" s="8"/>
+      <c r="B115" s="17"/>
+      <c r="C115" s="67"/>
+      <c r="D115" s="17"/>
+      <c r="E115" s="73"/>
+      <c r="F115" s="17"/>
+      <c r="G115" s="17"/>
+      <c r="H115" s="17"/>
       <c r="I115"/>
-      <c r="J115" s="8"/>
-      <c r="K115" s="8"/>
+      <c r="J115" s="17"/>
+      <c r="K115" s="17"/>
     </row>
     <row r="116" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="16"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="98"/>
-      <c r="D116" s="8"/>
-      <c r="E116" s="101"/>
-      <c r="F116" s="8"/>
-      <c r="G116" s="8"/>
-      <c r="H116" s="8"/>
+      <c r="B116" s="17"/>
+      <c r="C116" s="67"/>
+      <c r="D116" s="17"/>
+      <c r="E116" s="73"/>
+      <c r="F116" s="17"/>
+      <c r="G116" s="17"/>
+      <c r="H116" s="17"/>
       <c r="I116"/>
-      <c r="J116" s="8"/>
-      <c r="K116" s="8"/>
+      <c r="J116" s="17"/>
+      <c r="K116" s="17"/>
     </row>
     <row r="117" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="16"/>
-      <c r="B117" s="8"/>
-      <c r="C117" s="98"/>
-      <c r="D117" s="8"/>
-      <c r="E117" s="101"/>
-      <c r="F117" s="8"/>
-      <c r="G117" s="8"/>
-      <c r="H117" s="8"/>
+      <c r="B117" s="17"/>
+      <c r="C117" s="67"/>
+      <c r="D117" s="17"/>
+      <c r="E117" s="73"/>
+      <c r="F117" s="17"/>
+      <c r="G117" s="17"/>
+      <c r="H117" s="17"/>
       <c r="I117"/>
-      <c r="J117" s="8"/>
-      <c r="K117" s="8"/>
+      <c r="J117" s="17"/>
+      <c r="K117" s="17"/>
     </row>
     <row r="118" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="16"/>
-      <c r="B118" s="8"/>
-      <c r="C118" s="98"/>
-      <c r="D118" s="8"/>
-      <c r="E118" s="101"/>
-      <c r="F118" s="8"/>
-      <c r="G118" s="8"/>
-      <c r="H118" s="8"/>
+      <c r="B118" s="17"/>
+      <c r="C118" s="67"/>
+      <c r="D118" s="17"/>
+      <c r="E118" s="73"/>
+      <c r="F118" s="17"/>
+      <c r="G118" s="17"/>
+      <c r="H118" s="17"/>
       <c r="I118"/>
-      <c r="J118" s="8"/>
-      <c r="K118" s="8"/>
+      <c r="J118" s="17"/>
+      <c r="K118" s="17"/>
     </row>
     <row r="119" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="16"/>
-      <c r="B119" s="8"/>
-      <c r="C119" s="98"/>
-      <c r="D119" s="8"/>
-      <c r="E119" s="101"/>
-      <c r="F119" s="8"/>
-      <c r="G119" s="8"/>
-      <c r="H119" s="8"/>
+      <c r="B119" s="17"/>
+      <c r="C119" s="67"/>
+      <c r="D119" s="17"/>
+      <c r="E119" s="73"/>
+      <c r="F119" s="17"/>
+      <c r="G119" s="17"/>
+      <c r="H119" s="17"/>
       <c r="I119"/>
-      <c r="J119"/>
-      <c r="K119" s="8"/>
+      <c r="J119" s="17"/>
+      <c r="K119" s="17"/>
     </row>
     <row r="120" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="16"/>
       <c r="B120" s="8"/>
-      <c r="C120" s="98"/>
+      <c r="C120" s="68"/>
       <c r="D120" s="8"/>
-      <c r="E120" s="101"/>
+      <c r="E120" s="71"/>
       <c r="F120" s="8"/>
       <c r="G120" s="8"/>
       <c r="H120" s="8"/>
@@ -4559,9 +4816,9 @@
     <row r="121" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="16"/>
       <c r="B121" s="8"/>
-      <c r="C121" s="98"/>
+      <c r="C121" s="68"/>
       <c r="D121" s="8"/>
-      <c r="E121" s="101"/>
+      <c r="E121" s="71"/>
       <c r="F121" s="8"/>
       <c r="G121" s="8"/>
       <c r="H121" s="8"/>
@@ -4572,9 +4829,9 @@
     <row r="122" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="16"/>
       <c r="B122" s="8"/>
-      <c r="C122" s="98"/>
+      <c r="C122" s="68"/>
       <c r="D122" s="8"/>
-      <c r="E122" s="101"/>
+      <c r="E122" s="71"/>
       <c r="F122" s="8"/>
       <c r="G122" s="8"/>
       <c r="H122" s="8"/>
@@ -4585,9 +4842,9 @@
     <row r="123" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="16"/>
       <c r="B123" s="8"/>
-      <c r="C123" s="98"/>
+      <c r="C123" s="68"/>
       <c r="D123" s="8"/>
-      <c r="E123" s="101"/>
+      <c r="E123" s="71"/>
       <c r="F123" s="8"/>
       <c r="G123" s="8"/>
       <c r="H123" s="8"/>
@@ -4598,9 +4855,9 @@
     <row r="124" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="16"/>
       <c r="B124" s="8"/>
-      <c r="C124" s="98"/>
+      <c r="C124" s="68"/>
       <c r="D124" s="8"/>
-      <c r="E124" s="101"/>
+      <c r="E124" s="71"/>
       <c r="F124" s="8"/>
       <c r="G124" s="8"/>
       <c r="H124" s="8"/>
@@ -4611,9 +4868,9 @@
     <row r="125" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="16"/>
       <c r="B125" s="8"/>
-      <c r="C125" s="98"/>
+      <c r="C125" s="68"/>
       <c r="D125" s="8"/>
-      <c r="E125" s="101"/>
+      <c r="E125" s="71"/>
       <c r="F125" s="8"/>
       <c r="G125" s="8"/>
       <c r="H125" s="8"/>
@@ -4624,9 +4881,9 @@
     <row r="126" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="16"/>
       <c r="B126" s="8"/>
-      <c r="C126" s="98"/>
+      <c r="C126" s="68"/>
       <c r="D126" s="8"/>
-      <c r="E126" s="101"/>
+      <c r="E126" s="71"/>
       <c r="F126" s="8"/>
       <c r="G126" s="8"/>
       <c r="H126" s="8"/>
@@ -4637,22 +4894,22 @@
     <row r="127" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="16"/>
       <c r="B127" s="8"/>
-      <c r="C127" s="98"/>
+      <c r="C127" s="68"/>
       <c r="D127" s="8"/>
-      <c r="E127" s="101"/>
+      <c r="E127" s="71"/>
       <c r="F127" s="8"/>
       <c r="G127" s="8"/>
       <c r="H127" s="8"/>
       <c r="I127"/>
-      <c r="J127" s="8"/>
+      <c r="J127"/>
       <c r="K127" s="8"/>
     </row>
     <row r="128" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="16"/>
       <c r="B128" s="8"/>
-      <c r="C128" s="98"/>
+      <c r="C128" s="68"/>
       <c r="D128" s="8"/>
-      <c r="E128" s="101"/>
+      <c r="E128" s="71"/>
       <c r="F128" s="8"/>
       <c r="G128" s="8"/>
       <c r="H128" s="8"/>
@@ -4663,9 +4920,9 @@
     <row r="129" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="16"/>
       <c r="B129" s="8"/>
-      <c r="C129" s="98"/>
+      <c r="C129" s="68"/>
       <c r="D129" s="8"/>
-      <c r="E129" s="101"/>
+      <c r="E129" s="71"/>
       <c r="F129" s="8"/>
       <c r="G129" s="8"/>
       <c r="H129" s="8"/>
@@ -4676,9 +4933,9 @@
     <row r="130" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="16"/>
       <c r="B130" s="8"/>
-      <c r="C130" s="98"/>
+      <c r="C130" s="68"/>
       <c r="D130" s="8"/>
-      <c r="E130" s="101"/>
+      <c r="E130" s="71"/>
       <c r="F130" s="8"/>
       <c r="G130" s="8"/>
       <c r="H130" s="8"/>
@@ -4689,9 +4946,9 @@
     <row r="131" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="16"/>
       <c r="B131" s="8"/>
-      <c r="C131" s="98"/>
+      <c r="C131" s="68"/>
       <c r="D131" s="8"/>
-      <c r="E131" s="101"/>
+      <c r="E131" s="71"/>
       <c r="F131" s="8"/>
       <c r="G131" s="8"/>
       <c r="H131" s="8"/>
@@ -4702,9 +4959,9 @@
     <row r="132" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="16"/>
       <c r="B132" s="8"/>
-      <c r="C132" s="98"/>
+      <c r="C132" s="68"/>
       <c r="D132" s="8"/>
-      <c r="E132" s="101"/>
+      <c r="E132" s="71"/>
       <c r="F132" s="8"/>
       <c r="G132" s="8"/>
       <c r="H132" s="8"/>
@@ -4715,9 +4972,9 @@
     <row r="133" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="16"/>
       <c r="B133" s="8"/>
-      <c r="C133" s="98"/>
+      <c r="C133" s="68"/>
       <c r="D133" s="8"/>
-      <c r="E133" s="101"/>
+      <c r="E133" s="71"/>
       <c r="F133" s="8"/>
       <c r="G133" s="8"/>
       <c r="H133" s="8"/>
@@ -4728,9 +4985,9 @@
     <row r="134" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="16"/>
       <c r="B134" s="8"/>
-      <c r="C134" s="98"/>
+      <c r="C134" s="68"/>
       <c r="D134" s="8"/>
-      <c r="E134" s="101"/>
+      <c r="E134" s="71"/>
       <c r="F134" s="8"/>
       <c r="G134" s="8"/>
       <c r="H134" s="8"/>
@@ -4741,9 +4998,9 @@
     <row r="135" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="16"/>
       <c r="B135" s="8"/>
-      <c r="C135" s="98"/>
+      <c r="C135" s="68"/>
       <c r="D135" s="8"/>
-      <c r="E135" s="101"/>
+      <c r="E135" s="71"/>
       <c r="F135" s="8"/>
       <c r="G135" s="8"/>
       <c r="H135" s="8"/>
@@ -4754,9 +5011,9 @@
     <row r="136" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="16"/>
       <c r="B136" s="8"/>
-      <c r="C136" s="98"/>
+      <c r="C136" s="68"/>
       <c r="D136" s="8"/>
-      <c r="E136" s="101"/>
+      <c r="E136" s="71"/>
       <c r="F136" s="8"/>
       <c r="G136" s="8"/>
       <c r="H136" s="8"/>
@@ -4767,9 +5024,9 @@
     <row r="137" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="16"/>
       <c r="B137" s="8"/>
-      <c r="C137" s="98"/>
+      <c r="C137" s="68"/>
       <c r="D137" s="8"/>
-      <c r="E137" s="101"/>
+      <c r="E137" s="71"/>
       <c r="F137" s="8"/>
       <c r="G137" s="8"/>
       <c r="H137" s="8"/>
@@ -4777,108 +5034,116 @@
       <c r="J137" s="8"/>
       <c r="K137" s="8"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="16"/>
       <c r="B138" s="8"/>
-      <c r="C138" s="98"/>
+      <c r="C138" s="68"/>
       <c r="D138" s="8"/>
-      <c r="E138" s="101"/>
+      <c r="E138" s="71"/>
       <c r="F138" s="8"/>
       <c r="G138" s="8"/>
       <c r="H138" s="8"/>
+      <c r="I138"/>
       <c r="J138" s="8"/>
       <c r="K138" s="8"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="16"/>
       <c r="B139" s="8"/>
-      <c r="C139" s="98"/>
+      <c r="C139" s="68"/>
       <c r="D139" s="8"/>
-      <c r="E139" s="101"/>
+      <c r="E139" s="71"/>
       <c r="F139" s="8"/>
       <c r="G139" s="8"/>
       <c r="H139" s="8"/>
+      <c r="I139"/>
       <c r="J139" s="8"/>
       <c r="K139" s="8"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="16"/>
-      <c r="B140" s="17"/>
-      <c r="C140" s="97"/>
-      <c r="D140" s="17"/>
-      <c r="E140" s="103"/>
-      <c r="F140" s="17"/>
-      <c r="G140" s="17"/>
-      <c r="H140" s="17"/>
-      <c r="J140" s="17"/>
-      <c r="K140" s="17"/>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B140" s="8"/>
+      <c r="C140" s="68"/>
+      <c r="D140" s="8"/>
+      <c r="E140" s="71"/>
+      <c r="F140" s="8"/>
+      <c r="G140" s="8"/>
+      <c r="H140" s="8"/>
+      <c r="I140"/>
+      <c r="J140" s="8"/>
+      <c r="K140" s="8"/>
+    </row>
+    <row r="141" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="16"/>
       <c r="B141" s="8"/>
-      <c r="C141" s="98"/>
+      <c r="C141" s="68"/>
       <c r="D141" s="8"/>
-      <c r="E141" s="101"/>
+      <c r="E141" s="71"/>
       <c r="F141" s="8"/>
       <c r="G141" s="8"/>
       <c r="H141" s="8"/>
+      <c r="I141"/>
       <c r="J141" s="8"/>
       <c r="K141" s="8"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="16"/>
       <c r="B142" s="8"/>
-      <c r="C142" s="98"/>
+      <c r="C142" s="68"/>
       <c r="D142" s="8"/>
-      <c r="E142" s="101"/>
+      <c r="E142" s="71"/>
       <c r="F142" s="8"/>
       <c r="G142" s="8"/>
       <c r="H142" s="8"/>
+      <c r="I142"/>
       <c r="J142" s="8"/>
       <c r="K142" s="8"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="16"/>
       <c r="B143" s="8"/>
-      <c r="C143" s="98"/>
+      <c r="C143" s="68"/>
       <c r="D143" s="8"/>
-      <c r="E143" s="101"/>
+      <c r="E143" s="71"/>
       <c r="F143" s="8"/>
       <c r="G143" s="8"/>
       <c r="H143" s="8"/>
+      <c r="I143"/>
       <c r="J143" s="8"/>
       <c r="K143" s="8"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="16"/>
       <c r="B144" s="8"/>
-      <c r="C144" s="98"/>
+      <c r="C144" s="68"/>
       <c r="D144" s="8"/>
-      <c r="E144" s="101"/>
+      <c r="E144" s="71"/>
       <c r="F144" s="8"/>
       <c r="G144" s="8"/>
       <c r="H144" s="8"/>
+      <c r="I144"/>
       <c r="J144" s="8"/>
       <c r="K144" s="8"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="16"/>
       <c r="B145" s="8"/>
-      <c r="C145" s="98"/>
+      <c r="C145" s="68"/>
       <c r="D145" s="8"/>
-      <c r="E145" s="101"/>
+      <c r="E145" s="71"/>
       <c r="F145" s="8"/>
       <c r="G145" s="8"/>
       <c r="H145" s="8"/>
+      <c r="I145"/>
       <c r="J145" s="8"/>
       <c r="K145" s="8"/>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" s="16"/>
       <c r="B146" s="8"/>
-      <c r="C146" s="98"/>
+      <c r="C146" s="68"/>
       <c r="D146" s="8"/>
-      <c r="E146" s="101"/>
+      <c r="E146" s="71"/>
       <c r="F146" s="8"/>
       <c r="G146" s="8"/>
       <c r="H146" s="8"/>
@@ -4888,9 +5153,9 @@
     <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" s="16"/>
       <c r="B147" s="8"/>
-      <c r="C147" s="98"/>
+      <c r="C147" s="68"/>
       <c r="D147" s="8"/>
-      <c r="E147" s="101"/>
+      <c r="E147" s="71"/>
       <c r="F147" s="8"/>
       <c r="G147" s="8"/>
       <c r="H147" s="8"/>
@@ -4899,34 +5164,34 @@
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" s="16"/>
-      <c r="B148" s="8"/>
-      <c r="C148" s="98"/>
-      <c r="D148" s="8"/>
-      <c r="E148" s="101"/>
-      <c r="F148" s="8"/>
-      <c r="G148" s="8"/>
-      <c r="H148" s="8"/>
-      <c r="J148" s="8"/>
-      <c r="K148" s="8"/>
+      <c r="B148" s="17"/>
+      <c r="C148" s="67"/>
+      <c r="D148" s="17"/>
+      <c r="E148" s="73"/>
+      <c r="F148" s="17"/>
+      <c r="G148" s="17"/>
+      <c r="H148" s="17"/>
+      <c r="J148" s="17"/>
+      <c r="K148" s="17"/>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" s="16"/>
       <c r="B149" s="8"/>
-      <c r="C149" s="98"/>
+      <c r="C149" s="68"/>
       <c r="D149" s="8"/>
-      <c r="E149" s="101"/>
+      <c r="E149" s="71"/>
       <c r="F149" s="8"/>
       <c r="G149" s="8"/>
       <c r="H149" s="8"/>
       <c r="J149" s="8"/>
       <c r="K149" s="8"/>
     </row>
-    <row r="150" spans="1:11" ht="159" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" s="16"/>
       <c r="B150" s="8"/>
-      <c r="C150" s="98"/>
+      <c r="C150" s="68"/>
       <c r="D150" s="8"/>
-      <c r="E150" s="101"/>
+      <c r="E150" s="71"/>
       <c r="F150" s="8"/>
       <c r="G150" s="8"/>
       <c r="H150" s="8"/>
@@ -4936,9 +5201,9 @@
     <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" s="16"/>
       <c r="B151" s="8"/>
-      <c r="C151" s="98"/>
+      <c r="C151" s="68"/>
       <c r="D151" s="8"/>
-      <c r="E151" s="101"/>
+      <c r="E151" s="71"/>
       <c r="F151" s="8"/>
       <c r="G151" s="8"/>
       <c r="H151" s="8"/>
@@ -4948,17 +5213,113 @@
     <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" s="16"/>
       <c r="B152" s="8"/>
-      <c r="C152" s="98"/>
+      <c r="C152" s="68"/>
       <c r="D152" s="8"/>
-      <c r="E152" s="101"/>
+      <c r="E152" s="71"/>
       <c r="F152" s="8"/>
       <c r="G152" s="8"/>
       <c r="H152" s="8"/>
-      <c r="J152" s="7"/>
+      <c r="J152" s="8"/>
       <c r="K152" s="8"/>
     </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A153" s="16"/>
+      <c r="B153" s="8"/>
+      <c r="C153" s="68"/>
+      <c r="D153" s="8"/>
+      <c r="E153" s="71"/>
+      <c r="F153" s="8"/>
+      <c r="G153" s="8"/>
+      <c r="H153" s="8"/>
+      <c r="J153" s="8"/>
+      <c r="K153" s="8"/>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A154" s="16"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="68"/>
+      <c r="D154" s="8"/>
+      <c r="E154" s="71"/>
+      <c r="F154" s="8"/>
+      <c r="G154" s="8"/>
+      <c r="H154" s="8"/>
+      <c r="J154" s="8"/>
+      <c r="K154" s="8"/>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A155" s="16"/>
+      <c r="B155" s="8"/>
+      <c r="C155" s="68"/>
+      <c r="D155" s="8"/>
+      <c r="E155" s="71"/>
+      <c r="F155" s="8"/>
+      <c r="G155" s="8"/>
+      <c r="H155" s="8"/>
+      <c r="J155" s="8"/>
+      <c r="K155" s="8"/>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A156" s="16"/>
+      <c r="B156" s="8"/>
+      <c r="C156" s="68"/>
+      <c r="D156" s="8"/>
+      <c r="E156" s="71"/>
+      <c r="F156" s="8"/>
+      <c r="G156" s="8"/>
+      <c r="H156" s="8"/>
+      <c r="J156" s="8"/>
+      <c r="K156" s="8"/>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A157" s="16"/>
+      <c r="B157" s="8"/>
+      <c r="C157" s="68"/>
+      <c r="D157" s="8"/>
+      <c r="E157" s="71"/>
+      <c r="F157" s="8"/>
+      <c r="G157" s="8"/>
+      <c r="H157" s="8"/>
+      <c r="J157" s="8"/>
+      <c r="K157" s="8"/>
+    </row>
+    <row r="158" spans="1:11" ht="159" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="16"/>
+      <c r="B158" s="8"/>
+      <c r="C158" s="68"/>
+      <c r="D158" s="8"/>
+      <c r="E158" s="71"/>
+      <c r="F158" s="8"/>
+      <c r="G158" s="8"/>
+      <c r="H158" s="8"/>
+      <c r="J158" s="8"/>
+      <c r="K158" s="8"/>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A159" s="16"/>
+      <c r="B159" s="8"/>
+      <c r="C159" s="68"/>
+      <c r="D159" s="8"/>
+      <c r="E159" s="71"/>
+      <c r="F159" s="8"/>
+      <c r="G159" s="8"/>
+      <c r="H159" s="8"/>
+      <c r="J159" s="8"/>
+      <c r="K159" s="8"/>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A160" s="16"/>
+      <c r="B160" s="8"/>
+      <c r="C160" s="68"/>
+      <c r="D160" s="8"/>
+      <c r="E160" s="71"/>
+      <c r="F160" s="8"/>
+      <c r="G160" s="8"/>
+      <c r="H160" s="8"/>
+      <c r="J160" s="7"/>
+      <c r="K160" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A7:K152"/>
+  <autoFilter ref="A7:K160"/>
   <mergeCells count="13">
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="A1:K2"/>
@@ -5004,109 +5365,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
     </row>
     <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
+      <c r="A2" s="98"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
     </row>
     <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="84" t="s">
+      <c r="B3" s="99"/>
+      <c r="C3" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="84"/>
+      <c r="D3" s="100"/>
       <c r="E3" s="48" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
     </row>
     <row r="4" spans="1:11" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="88" t="s">
+      <c r="B4" s="103"/>
+      <c r="C4" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="88"/>
+      <c r="D4" s="104"/>
       <c r="E4" s="49" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
     </row>
     <row r="5" spans="1:11" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="88" t="s">
+      <c r="B5" s="103"/>
+      <c r="C5" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="88"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="86"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
+      <c r="K5" s="102"/>
     </row>
     <row r="6" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="76"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="76" t="s">
+      <c r="A6" s="92"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="78"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="79" t="s">
+      <c r="D6" s="94"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="80"/>
-      <c r="H6" s="81" t="s">
+      <c r="G6" s="96"/>
+      <c r="H6" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="97"/>
       <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>